<commit_message>
sem brinde iniciante, criado n ok
</commit_message>
<xml_diff>
--- a/data/AutoVC.xlsx
+++ b/data/AutoVC.xlsx
@@ -15,8 +15,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Testes!$A$1:$AG$47</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT([0]!LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3" hidden="1"><![CDATA[REPT(LOCAL_YEAR_FORMAT,4)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_MONTH_FORMAT,2)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_DAY_FORMAT,2)&" "&REPT(LOCAL_HOUR_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT(LOCAL_MINUTE_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT([0]!LOCAL_SECOND_FORMAT,2)]]></definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1"><![CDATA[REPT(LOCAL_YEAR_FORMAT,4)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_MONTH_FORMAT,2)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_DAY_FORMAT,2)&" "&REPT(LOCAL_HOUR_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT(LOCAL_MINUTE_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT(LOCAL_SECOND_FORMAT,2)]]></definedName>
     <definedName name="LOCAL_SECOND_FORMAT" hidden="1">" "</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1665" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="339">
   <si>
     <t>Telefone</t>
   </si>
@@ -1107,10 +1107,10 @@
     <t>Falha ao logar com email</t>
   </si>
   <si>
-    <t>00:01:32</t>
-  </si>
-  <si>
     <t>00:01:43</t>
+  </si>
+  <si>
+    <t>00:00:05</t>
   </si>
 </sst>
 </file>
@@ -1579,7 +1579,7 @@
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1773,6 +1773,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8418,43 +8419,43 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" style="10" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="131.42578125" style="75" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.85546875" style="31" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="43.5703125" style="10" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="35.7109375" style="10" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.7109375" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.7109375" style="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="12.7109375" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="26.85546875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.140625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23.28515625" style="10" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="8.28515625" style="10" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="23.5703125" style="10" customWidth="1" collapsed="1"/>
-    <col min="19" max="20" width="15" style="10" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="15.140625" style="10" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.28515625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="23.85546875" style="10" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="24.5703125" style="10" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="19.140625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="17.5703125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="25.7109375" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="17.7109375" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="19.28515625" style="10" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="14" style="14" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.28515625" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="16384" width="9.140625" style="14" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="10" width="7.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="10" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="75" width="131.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="31" width="11.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="10" width="43.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="10" width="35.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="10" width="11.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="10" width="11.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="10" width="14.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="8" width="10.7109375" collapsed="true"/>
+    <col min="11" max="12" bestFit="true" customWidth="true" style="10" width="12.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="10" width="26.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="10" width="15.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="10" width="23.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="10" width="8.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="10" width="12.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="10" width="23.5703125" collapsed="true"/>
+    <col min="19" max="20" customWidth="true" style="10" width="15.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="10" width="12.0" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="10" width="15.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="10" width="13.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="10" width="23.85546875" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="10" width="24.5703125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="10" width="19.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="10" width="17.5703125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="10" width="25.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="10" width="17.7109375" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="10" width="19.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="10" width="24.0" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="14" width="14.0" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="14" width="15.28515625" collapsed="true"/>
+    <col min="34" max="16384" style="14" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" s="13" customFormat="1">
@@ -8581,7 +8582,7 @@
         <v>247</v>
       </c>
       <c r="H2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I2" t="s">
         <v>329</v>
@@ -8666,23 +8667,23 @@
       <c r="B3" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="97" t="s">
+      <c r="C3" s="107" t="s">
         <v>147</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>117</v>
       </c>
       <c r="F3" t="s">
-        <v>336</v>
+        <v>117</v>
       </c>
       <c r="G3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H3" t="s">
-        <v>337</v>
+        <v>267</v>
       </c>
       <c r="I3" t="s">
         <v>329</v>
@@ -9977,22 +9978,22 @@
         <v>334</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>117</v>
       </c>
       <c r="F16" t="s">
-        <v>117</v>
+        <v>328</v>
       </c>
       <c r="G16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H16" t="s">
-        <v>319</v>
+        <v>338</v>
       </c>
       <c r="I16" t="s">
-        <v>301</v>
+        <v>329</v>
       </c>
       <c r="J16" t="s">
         <v>140</v>
@@ -13002,43 +13003,43 @@
       <c r="J47" s="22"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
-      <c r="M47" s="110" t="s">
+      <c r="M47" s="111" t="s">
         <v>157</v>
       </c>
-      <c r="N47" s="110"/>
-      <c r="O47" s="111" t="s">
+      <c r="N47" s="111"/>
+      <c r="O47" s="112" t="s">
         <v>195</v>
       </c>
-      <c r="P47" s="111"/>
-      <c r="Q47" s="111"/>
-      <c r="R47" s="111"/>
-      <c r="S47" s="111"/>
-      <c r="T47" s="111"/>
-      <c r="U47" s="111"/>
-      <c r="V47" s="113" t="s">
+      <c r="P47" s="112"/>
+      <c r="Q47" s="112"/>
+      <c r="R47" s="112"/>
+      <c r="S47" s="112"/>
+      <c r="T47" s="112"/>
+      <c r="U47" s="112"/>
+      <c r="V47" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="W47" s="113"/>
-      <c r="X47" s="109" t="s">
+      <c r="W47" s="114"/>
+      <c r="X47" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="Y47" s="109"/>
-      <c r="Z47" s="112" t="s">
+      <c r="Y47" s="110"/>
+      <c r="Z47" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="AA47" s="112"/>
+      <c r="AA47" s="113"/>
       <c r="AB47" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="AC47" s="114" t="s">
+      <c r="AC47" s="115" t="s">
         <v>218</v>
       </c>
-      <c r="AD47" s="115"/>
-      <c r="AE47" s="116"/>
-      <c r="AF47" s="107" t="s">
+      <c r="AD47" s="116"/>
+      <c r="AE47" s="117"/>
+      <c r="AF47" s="108" t="s">
         <v>155</v>
       </c>
-      <c r="AG47" s="108"/>
+      <c r="AG47" s="109"/>
     </row>
     <row r="49" spans="2:35">
       <c r="B49" s="87" t="s">
@@ -15888,16 +15889,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5703125" style="39" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" style="39" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="15.85546875" style="39" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.28515625" style="39" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="1.5703125" style="39" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.85546875" style="39" customWidth="1" collapsed="1"/>
-    <col min="9" max="12" width="13.42578125" style="39" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="1.5703125" style="39" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="9.140625" style="39" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="39" width="1.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="39" width="14.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="39" width="15.85546875" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" style="39" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="39" width="19.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="39" width="1.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="39" width="15.85546875" collapsed="true"/>
+    <col min="9" max="12" customWidth="true" style="39" width="13.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="39" width="1.5703125" collapsed="true"/>
+    <col min="14" max="16384" style="39" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="7.5" customHeight="1">
@@ -15925,11 +15926,11 @@
       <c r="E2" s="43"/>
       <c r="F2" s="43"/>
       <c r="G2" s="43"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="118"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
       <c r="M2" s="46"/>
     </row>
     <row r="3" spans="1:13" ht="7.5" customHeight="1">
@@ -15949,21 +15950,21 @@
     </row>
     <row r="4" spans="1:13" s="63" customFormat="1" ht="26.25" customHeight="1">
       <c r="A4" s="62"/>
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="120" t="s">
         <v>171</v>
       </c>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
       <c r="G4" s="62"/>
-      <c r="H4" s="119" t="s">
+      <c r="H4" s="120" t="s">
         <v>172</v>
       </c>
-      <c r="I4" s="119"/>
-      <c r="J4" s="119"/>
-      <c r="K4" s="119"/>
-      <c r="L4" s="119"/>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="120"/>
       <c r="M4" s="62"/>
     </row>
     <row r="5" spans="1:13" ht="15">
@@ -15983,12 +15984,12 @@
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1">
       <c r="A6" s="46"/>
-      <c r="B6" s="121" t="s">
+      <c r="B6" s="122" t="s">
         <v>188</v>
       </c>
-      <c r="C6" s="120"/>
-      <c r="D6" s="120"/>
-      <c r="E6" s="120"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
       <c r="F6" s="53">
         <f>(J11+K11)/I11</f>
         <v>0.90697674418604646</v>
@@ -16011,10 +16012,10 @@
     </row>
     <row r="7" spans="1:13" ht="25.5">
       <c r="A7" s="46"/>
-      <c r="B7" s="121"/>
-      <c r="C7" s="120"/>
-      <c r="D7" s="120"/>
-      <c r="E7" s="120"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="121"/>
+      <c r="D7" s="121"/>
+      <c r="E7" s="121"/>
       <c r="F7" s="54" t="s">
         <v>186</v>
       </c>
@@ -16045,9 +16046,9 @@
         <f>COUNTIF(Testes!A3:A46,"&lt;&gt;"&amp;"")</f>
         <v>44</v>
       </c>
-      <c r="C8" s="120"/>
-      <c r="D8" s="120"/>
-      <c r="E8" s="120"/>
+      <c r="C8" s="121"/>
+      <c r="D8" s="121"/>
+      <c r="E8" s="121"/>
       <c r="F8" s="56"/>
       <c r="G8" s="46"/>
       <c r="H8" s="50" t="s">
@@ -16073,9 +16074,9 @@
     <row r="9" spans="1:13" ht="23.25">
       <c r="A9" s="46"/>
       <c r="B9" s="57"/>
-      <c r="C9" s="120"/>
-      <c r="D9" s="120"/>
-      <c r="E9" s="120"/>
+      <c r="C9" s="121"/>
+      <c r="D9" s="121"/>
+      <c r="E9" s="121"/>
       <c r="F9" s="58">
         <f>SUM(Testes!H3:H46)</f>
         <v>0</v>
@@ -16116,7 +16117,7 @@
         <f>K11</f>
         <v>8</v>
       </c>
-      <c r="F10" s="117" t="s">
+      <c r="F10" s="118" t="s">
         <v>189</v>
       </c>
       <c r="G10" s="47"/>
@@ -16139,7 +16140,7 @@
       <c r="E11" s="59" t="s">
         <v>174</v>
       </c>
-      <c r="F11" s="117"/>
+      <c r="F11" s="118"/>
       <c r="G11" s="47"/>
       <c r="H11" s="41" t="s">
         <v>185</v>
@@ -16241,9 +16242,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -16396,29 +16397,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" style="10" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.28515625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.85546875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.5703125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.140625" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.5703125" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.28515625" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.5703125" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.85546875" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8.5703125" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="3.42578125" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.5703125" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.5703125" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="24.5703125" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.85546875" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.85546875" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="20.140625" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="20.42578125" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="16384" width="9.140625" style="14" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="10" width="35.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="10" width="9.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="7.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="25.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="14" width="12.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="14" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="14" width="21.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="14" width="19.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="14" width="15.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="14" width="20.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="14" width="13.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="14" width="19.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="14" width="8.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="14" width="3.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="14" width="18.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="14" width="13.5703125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="14" width="12.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="14" width="24.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="14" width="13.85546875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="14" width="11.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="14" width="20.140625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="14" width="20.42578125" collapsed="true"/>
+    <col min="23" max="16384" style="14" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="13" customFormat="1">
@@ -16809,30 +16810,30 @@
       <c r="D32" s="12"/>
     </row>
     <row r="33" spans="1:22">
-      <c r="A33" s="122" t="s">
+      <c r="A33" s="123" t="s">
         <v>100</v>
       </c>
-      <c r="B33" s="122"/>
-      <c r="C33" s="122"/>
-      <c r="D33" s="122"/>
-      <c r="E33" s="122"/>
-      <c r="F33" s="122"/>
-      <c r="G33" s="122"/>
-      <c r="H33" s="122"/>
-      <c r="I33" s="122"/>
-      <c r="J33" s="122"/>
-      <c r="K33" s="122"/>
-      <c r="L33" s="122"/>
-      <c r="M33" s="122"/>
-      <c r="N33" s="122"/>
-      <c r="O33" s="122"/>
-      <c r="P33" s="122"/>
-      <c r="Q33" s="122"/>
-      <c r="R33" s="122"/>
-      <c r="S33" s="122"/>
-      <c r="T33" s="122"/>
-      <c r="U33" s="122"/>
-      <c r="V33" s="122"/>
+      <c r="B33" s="123"/>
+      <c r="C33" s="123"/>
+      <c r="D33" s="123"/>
+      <c r="E33" s="123"/>
+      <c r="F33" s="123"/>
+      <c r="G33" s="123"/>
+      <c r="H33" s="123"/>
+      <c r="I33" s="123"/>
+      <c r="J33" s="123"/>
+      <c r="K33" s="123"/>
+      <c r="L33" s="123"/>
+      <c r="M33" s="123"/>
+      <c r="N33" s="123"/>
+      <c r="O33" s="123"/>
+      <c r="P33" s="123"/>
+      <c r="Q33" s="123"/>
+      <c r="R33" s="123"/>
+      <c r="S33" s="123"/>
+      <c r="T33" s="123"/>
+      <c r="U33" s="123"/>
+      <c r="V33" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -16872,11 +16873,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">

</xml_diff>

<commit_message>
novos testes cards, brindes e cupons ordenados.
</commit_message>
<xml_diff>
--- a/data/AutoVC.xlsx
+++ b/data/AutoVC.xlsx
@@ -1079,9 +1079,6 @@
     <t>00:01:34</t>
   </si>
   <si>
-    <t>00:00:42</t>
-  </si>
-  <si>
     <t>1.0.0.1659227</t>
   </si>
   <si>
@@ -1245,6 +1242,9 @@
   </si>
   <si>
     <t>00:01:43</t>
+  </si>
+  <si>
+    <t>30/07/2021</t>
   </si>
 </sst>
 </file>
@@ -9652,7 +9652,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9815,7 +9815,7 @@
         <v>238</v>
       </c>
       <c r="H2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I2" t="s">
         <v>303</v>
@@ -9869,7 +9869,7 @@
         <v>134</v>
       </c>
       <c r="Z2" s="92" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AA2" s="10">
         <v>44096</v>
@@ -9901,7 +9901,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="93" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D3" t="s">
         <v>131</v>
@@ -10002,7 +10002,7 @@
         <v>301</v>
       </c>
       <c r="C4" s="93" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D4" t="s">
         <v>131</v>
@@ -10017,10 +10017,10 @@
         <v>238</v>
       </c>
       <c r="H4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I4" t="s">
-        <v>303</v>
+        <v>378</v>
       </c>
       <c r="J4" t="s">
         <v>136</v>
@@ -10100,10 +10100,10 @@
         <v>227</v>
       </c>
       <c r="B5" s="105" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C5" s="93" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D5" t="s">
         <v>131</v>
@@ -10132,11 +10132,11 @@
       <c r="L5" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="M5" s="90" t="s">
-        <v>300</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>260</v>
+      <c r="M5" s="76" t="s">
+        <v>239</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="O5" s="7" t="s">
         <v>134</v>
@@ -13254,7 +13254,7 @@
         <v>238</v>
       </c>
       <c r="H37" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I37" t="s">
         <v>303</v>
@@ -13275,7 +13275,7 @@
         <v>134</v>
       </c>
       <c r="O37" s="79" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P37" s="7" t="s">
         <v>134</v>
@@ -13759,7 +13759,7 @@
         <v>238</v>
       </c>
       <c r="H42" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I42" t="s">
         <v>303</v>
@@ -13957,7 +13957,7 @@
         <v>238</v>
       </c>
       <c r="H44" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I44" t="s">
         <v>303</v>
@@ -14041,7 +14041,7 @@
         <v>215</v>
       </c>
       <c r="C45" s="75" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D45" t="s">
         <v>131</v>
@@ -14056,7 +14056,7 @@
         <v>237</v>
       </c>
       <c r="H45" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I45" t="s">
         <v>303</v>
@@ -14134,13 +14134,13 @@
     </row>
     <row r="46" spans="1:33">
       <c r="A46" s="14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B46" s="91" t="s">
         <v>214</v>
       </c>
       <c r="C46" s="75" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D46" t="s">
         <v>131</v>
@@ -14225,13 +14225,13 @@
     </row>
     <row r="47" spans="1:33">
       <c r="A47" s="14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B47" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="C47" s="103" t="s">
         <v>332</v>
-      </c>
-      <c r="C47" s="103" t="s">
-        <v>333</v>
       </c>
       <c r="D47" t="s">
         <v>131</v>
@@ -14326,13 +14326,13 @@
     </row>
     <row r="48" spans="1:33">
       <c r="A48" s="14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B48" s="103" t="s">
+        <v>350</v>
+      </c>
+      <c r="C48" s="103" t="s">
         <v>351</v>
-      </c>
-      <c r="C48" s="103" t="s">
-        <v>352</v>
       </c>
       <c r="D48"/>
       <c r="E48" s="5"/>
@@ -14367,13 +14367,13 @@
     </row>
     <row r="49" spans="1:33">
       <c r="A49" s="14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B49" s="103" t="s">
+        <v>352</v>
+      </c>
+      <c r="C49" s="103" t="s">
         <v>353</v>
-      </c>
-      <c r="C49" s="103" t="s">
-        <v>354</v>
       </c>
       <c r="D49"/>
       <c r="E49" s="5"/>
@@ -14408,13 +14408,13 @@
     </row>
     <row r="50" spans="1:33">
       <c r="A50" s="14" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B50" s="103" t="s">
+        <v>354</v>
+      </c>
+      <c r="C50" s="103" t="s">
         <v>355</v>
-      </c>
-      <c r="C50" s="103" t="s">
-        <v>356</v>
       </c>
       <c r="D50"/>
       <c r="E50" s="5"/>
@@ -14449,13 +14449,13 @@
     </row>
     <row r="51" spans="1:33">
       <c r="A51" s="14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B51" s="103" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C51" s="103" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D51"/>
       <c r="E51" s="5"/>
@@ -14493,10 +14493,10 @@
         <v>62</v>
       </c>
       <c r="B52" s="103" t="s">
+        <v>357</v>
+      </c>
+      <c r="C52" s="103" t="s">
         <v>358</v>
-      </c>
-      <c r="C52" s="103" t="s">
-        <v>359</v>
       </c>
       <c r="D52"/>
       <c r="E52" s="5"/>
@@ -14534,10 +14534,10 @@
         <v>63</v>
       </c>
       <c r="B53" s="103" t="s">
+        <v>359</v>
+      </c>
+      <c r="C53" s="103" t="s">
         <v>360</v>
-      </c>
-      <c r="C53" s="103" t="s">
-        <v>361</v>
       </c>
       <c r="D53"/>
       <c r="E53" s="5"/>
@@ -14572,13 +14572,13 @@
     </row>
     <row r="54" spans="1:33">
       <c r="A54" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B54" s="103" t="s">
+        <v>361</v>
+      </c>
+      <c r="C54" s="103" t="s">
         <v>362</v>
-      </c>
-      <c r="C54" s="103" t="s">
-        <v>363</v>
       </c>
       <c r="D54"/>
       <c r="E54" s="5"/>
@@ -14613,13 +14613,13 @@
     </row>
     <row r="55" spans="1:33">
       <c r="A55" s="14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B55" s="103" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C55" s="103" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D55"/>
       <c r="E55" s="5"/>
@@ -14654,13 +14654,13 @@
     </row>
     <row r="56" spans="1:33">
       <c r="A56" s="14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B56" s="103" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C56" s="103" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D56"/>
       <c r="E56" s="5"/>
@@ -14695,13 +14695,13 @@
     </row>
     <row r="57" spans="1:33">
       <c r="A57" s="14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B57" s="103" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C57" s="103" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D57"/>
       <c r="E57" s="5"/>
@@ -14736,13 +14736,13 @@
     </row>
     <row r="58" spans="1:33">
       <c r="A58" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B58" s="103" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C58" s="103" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D58"/>
       <c r="E58" s="5"/>
@@ -14777,13 +14777,13 @@
     </row>
     <row r="59" spans="1:33">
       <c r="A59" s="14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B59" s="103" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C59" s="103" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D59"/>
       <c r="E59" s="5"/>
@@ -14818,13 +14818,13 @@
     </row>
     <row r="60" spans="1:33">
       <c r="A60" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B60" s="103" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C60" s="103" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D60"/>
       <c r="E60" s="5"/>
@@ -14859,13 +14859,13 @@
     </row>
     <row r="61" spans="1:33">
       <c r="A61" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B61" s="103" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C61" s="103" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D61"/>
       <c r="E61" s="5"/>
@@ -14900,13 +14900,13 @@
     </row>
     <row r="62" spans="1:33">
       <c r="A62" s="14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B62" s="103" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C62" s="103" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D62"/>
       <c r="E62" s="5"/>
@@ -14941,13 +14941,13 @@
     </row>
     <row r="63" spans="1:33">
       <c r="A63" s="14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B63" s="103" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C63" s="103" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D63"/>
       <c r="E63" s="5"/>
@@ -14982,7 +14982,7 @@
     </row>
     <row r="64" spans="1:33">
       <c r="A64" s="14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B64" s="102"/>
       <c r="D64"/>
@@ -18310,11 +18310,10 @@
     <hyperlink ref="M21" r:id="rId6"/>
     <hyperlink ref="M36" r:id="rId7"/>
     <hyperlink ref="M45" r:id="rId8"/>
-    <hyperlink ref="M5" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
-  <legacyDrawing r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
teste captura brindes ok
</commit_message>
<xml_diff>
--- a/data/AutoVC.xlsx
+++ b/data/AutoVC.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2322" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2322" uniqueCount="422">
   <si>
     <t>Telefone</t>
   </si>
@@ -1247,15 +1247,9 @@
     <t>30/07/2021</t>
   </si>
   <si>
-    <t>Usuário sem viagem - Brindes</t>
-  </si>
-  <si>
     <t>Captura tela dos cards</t>
   </si>
   <si>
-    <t>Usuário sem viagem - Cupons</t>
-  </si>
-  <si>
     <t>Captura tela dos cupons</t>
   </si>
   <si>
@@ -1304,12 +1298,6 @@
     <t>28/07/2027</t>
   </si>
   <si>
-    <t>00:00:12</t>
-  </si>
-  <si>
-    <t>28/07/2028</t>
-  </si>
-  <si>
     <t>00:00:13</t>
   </si>
   <si>
@@ -1379,7 +1367,13 @@
     <t>Usuario sem viagem - Cards</t>
   </si>
   <si>
-    <t>00:00:42</t>
+    <t>Usuario sem viagem - Brindes</t>
+  </si>
+  <si>
+    <t>Usuario sem viagem - Cupons</t>
+  </si>
+  <si>
+    <t>00:00:38</t>
   </si>
 </sst>
 </file>
@@ -10954,9 +10948,9 @@
   <dimension ref="A1:AI82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
+      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15532,10 +15526,10 @@
         <v>335</v>
       </c>
       <c r="B47" s="105" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C47" s="105" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D47" t="s">
         <v>131</v>
@@ -15752,10 +15746,10 @@
         <v>237</v>
       </c>
       <c r="H49" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I49" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J49" t="s">
         <v>136</v>
@@ -15853,10 +15847,10 @@
         <v>237</v>
       </c>
       <c r="H50" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I50" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="J50" t="s">
         <v>136</v>
@@ -15954,10 +15948,10 @@
         <v>237</v>
       </c>
       <c r="H51" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I51" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J51" t="s">
         <v>136</v>
@@ -16055,10 +16049,10 @@
         <v>237</v>
       </c>
       <c r="H52" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I52" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J52" t="s">
         <v>136</v>
@@ -16156,10 +16150,10 @@
         <v>237</v>
       </c>
       <c r="H53" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I53" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="J53" t="s">
         <v>136</v>
@@ -16257,10 +16251,10 @@
         <v>237</v>
       </c>
       <c r="H54" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I54" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="J54" t="s">
         <v>136</v>
@@ -16340,10 +16334,10 @@
         <v>341</v>
       </c>
       <c r="B55" s="106" t="s">
+        <v>419</v>
+      </c>
+      <c r="C55" s="106" t="s">
         <v>379</v>
-      </c>
-      <c r="C55" s="106" t="s">
-        <v>380</v>
       </c>
       <c r="D55" t="s">
         <v>131</v>
@@ -16352,16 +16346,16 @@
         <v>113</v>
       </c>
       <c r="F55" t="s">
-        <v>297</v>
+        <v>113</v>
       </c>
       <c r="G55" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H55" t="s">
-        <v>398</v>
+        <v>421</v>
       </c>
       <c r="I55" t="s">
-        <v>399</v>
+        <v>378</v>
       </c>
       <c r="J55" t="s">
         <v>136</v>
@@ -16459,10 +16453,10 @@
         <v>237</v>
       </c>
       <c r="H56" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="I56" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="J56" t="s">
         <v>136</v>
@@ -16560,10 +16554,10 @@
         <v>237</v>
       </c>
       <c r="H57" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="I57" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="J57" t="s">
         <v>136</v>
@@ -16661,10 +16655,10 @@
         <v>237</v>
       </c>
       <c r="H58" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="I58" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="J58" t="s">
         <v>136</v>
@@ -16762,10 +16756,10 @@
         <v>237</v>
       </c>
       <c r="H59" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="I59" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="J59" t="s">
         <v>136</v>
@@ -16863,10 +16857,10 @@
         <v>237</v>
       </c>
       <c r="H60" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="I60" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="J60" t="s">
         <v>136</v>
@@ -16964,10 +16958,10 @@
         <v>237</v>
       </c>
       <c r="H61" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="I61" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="J61" t="s">
         <v>136</v>
@@ -17047,10 +17041,10 @@
         <v>348</v>
       </c>
       <c r="B62" s="105" t="s">
-        <v>381</v>
+        <v>420</v>
       </c>
       <c r="C62" s="105" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D62" t="s">
         <v>131</v>
@@ -17065,10 +17059,10 @@
         <v>237</v>
       </c>
       <c r="H62" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="I62" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="J62" t="s">
         <v>136</v>
@@ -17166,10 +17160,10 @@
         <v>237</v>
       </c>
       <c r="H63" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="I63" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="J63" t="s">
         <v>136</v>
@@ -17246,7 +17240,7 @@
     </row>
     <row r="64" spans="1:33">
       <c r="A64" s="14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B64" s="105" t="s">
         <v>369</v>
@@ -17267,10 +17261,10 @@
         <v>237</v>
       </c>
       <c r="H64" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="I64" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="J64" t="s">
         <v>136</v>
@@ -17347,7 +17341,7 @@
     </row>
     <row r="65" spans="1:35">
       <c r="A65" s="14" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B65" s="105" t="s">
         <v>370</v>
@@ -17368,10 +17362,10 @@
         <v>237</v>
       </c>
       <c r="H65" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="I65" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="J65" t="s">
         <v>136</v>
@@ -17448,7 +17442,7 @@
     </row>
     <row r="66" spans="1:35">
       <c r="A66" s="14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B66" s="105" t="s">
         <v>371</v>
@@ -17469,10 +17463,10 @@
         <v>237</v>
       </c>
       <c r="H66" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="I66" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="J66" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
teste captura cupons ok
</commit_message>
<xml_diff>
--- a/data/AutoVC.xlsx
+++ b/data/AutoVC.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2322" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2332" uniqueCount="423">
   <si>
     <t>Telefone</t>
   </si>
@@ -1334,12 +1334,6 @@
     <t>28/07/2034</t>
   </si>
   <si>
-    <t>00:00:19</t>
-  </si>
-  <si>
-    <t>28/07/2035</t>
-  </si>
-  <si>
     <t>00:00:20</t>
   </si>
   <si>
@@ -1371,6 +1365,15 @@
   </si>
   <si>
     <t>Usuario sem viagem - Cupons</t>
+  </si>
+  <si>
+    <t>00:00:36</t>
+  </si>
+  <si>
+    <t>00:00:32</t>
+  </si>
+  <si>
+    <t>00:00:33</t>
   </si>
   <si>
     <t>00:00:38</t>
@@ -10948,9 +10951,9 @@
   <dimension ref="A1:AI82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15526,7 +15529,7 @@
         <v>335</v>
       </c>
       <c r="B47" s="105" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C47" s="105" t="s">
         <v>379</v>
@@ -15544,7 +15547,7 @@
         <v>238</v>
       </c>
       <c r="H47" t="s">
-        <v>277</v>
+        <v>247</v>
       </c>
       <c r="I47" t="s">
         <v>378</v>
@@ -16334,7 +16337,7 @@
         <v>341</v>
       </c>
       <c r="B55" s="106" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C55" s="106" t="s">
         <v>379</v>
@@ -16352,7 +16355,7 @@
         <v>238</v>
       </c>
       <c r="H55" t="s">
-        <v>421</v>
+        <v>277</v>
       </c>
       <c r="I55" t="s">
         <v>378</v>
@@ -17041,7 +17044,7 @@
         <v>348</v>
       </c>
       <c r="B62" s="105" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C62" s="105" t="s">
         <v>380</v>
@@ -17053,16 +17056,16 @@
         <v>113</v>
       </c>
       <c r="F62" t="s">
-        <v>297</v>
+        <v>113</v>
       </c>
       <c r="G62" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H62" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
       <c r="I62" t="s">
-        <v>409</v>
+        <v>378</v>
       </c>
       <c r="J62" t="s">
         <v>136</v>
@@ -17160,10 +17163,10 @@
         <v>237</v>
       </c>
       <c r="H63" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I63" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="J63" t="s">
         <v>136</v>
@@ -17261,10 +17264,10 @@
         <v>237</v>
       </c>
       <c r="H64" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I64" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="J64" t="s">
         <v>136</v>
@@ -17362,10 +17365,10 @@
         <v>237</v>
       </c>
       <c r="H65" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I65" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="J65" t="s">
         <v>136</v>
@@ -17463,10 +17466,10 @@
         <v>237</v>
       </c>
       <c r="H66" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="I66" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="J66" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
teste login 3 viagens criado
</commit_message>
<xml_diff>
--- a/data/AutoVC.xlsx
+++ b/data/AutoVC.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2332" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2322" uniqueCount="424">
   <si>
     <t>Telefone</t>
   </si>
@@ -1367,16 +1367,19 @@
     <t>Usuario sem viagem - Cupons</t>
   </si>
   <si>
+    <t>00:00:38</t>
+  </si>
+  <si>
+    <t>Funcionalidade [Login Email Manipulado 3 viagens &lt;70] não encontrado</t>
+  </si>
+  <si>
+    <t>02/08/2021</t>
+  </si>
+  <si>
     <t>00:00:36</t>
   </si>
   <si>
-    <t>00:00:32</t>
-  </si>
-  <si>
-    <t>00:00:33</t>
-  </si>
-  <si>
-    <t>00:00:38</t>
+    <t>00:01:30</t>
   </si>
 </sst>
 </file>
@@ -10951,9 +10954,9 @@
   <dimension ref="A1:AI82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
+      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11419,10 +11422,10 @@
         <v>238</v>
       </c>
       <c r="H5" t="s">
-        <v>255</v>
+        <v>423</v>
       </c>
       <c r="I5" t="s">
-        <v>298</v>
+        <v>421</v>
       </c>
       <c r="J5" t="s">
         <v>136</v>
@@ -17062,7 +17065,7 @@
         <v>238</v>
       </c>
       <c r="H62" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="I62" t="s">
         <v>378</v>

</xml_diff>

<commit_message>
cadastro facebook e google na versão 1.0.0.1662005 ok
</commit_message>
<xml_diff>
--- a/data/AutoVC.xlsx
+++ b/data/AutoVC.xlsx
@@ -673,9 +673,6 @@
     <t>Realizar login utilizando Facebook</t>
   </si>
   <si>
-    <t>Atenção: as linhas destacadas em amarelo precisam ter a massa de dados alterada antes da execução</t>
-  </si>
-  <si>
     <t>CT36</t>
   </si>
   <si>
@@ -962,9 +959,6 @@
   </si>
   <si>
     <t>00:01:05</t>
-  </si>
-  <si>
-    <t>falha ao pular tour inicial</t>
   </si>
   <si>
     <t>00:01:02</t>
@@ -1058,9 +1052,6 @@
     <t>00:01:34</t>
   </si>
   <si>
-    <t>1.0.0.1659227</t>
-  </si>
-  <si>
     <t>https://autovc.page.link/GcZk</t>
   </si>
   <si>
@@ -1202,160 +1193,169 @@
     <t>Realizar login utilizando E-mail viagens em andamento</t>
   </si>
   <si>
+    <t>30/07/2021</t>
+  </si>
+  <si>
+    <t>Captura tela dos cards</t>
+  </si>
+  <si>
+    <t>Captura tela dos cupons</t>
+  </si>
+  <si>
+    <t>CT63</t>
+  </si>
+  <si>
+    <t>CT64</t>
+  </si>
+  <si>
+    <t>CT65</t>
+  </si>
+  <si>
+    <t>00:00:06</t>
+  </si>
+  <si>
+    <t>28/07/2022</t>
+  </si>
+  <si>
+    <t>00:00:07</t>
+  </si>
+  <si>
+    <t>28/07/2023</t>
+  </si>
+  <si>
+    <t>00:00:08</t>
+  </si>
+  <si>
+    <t>28/07/2024</t>
+  </si>
+  <si>
+    <t>00:00:09</t>
+  </si>
+  <si>
+    <t>28/07/2025</t>
+  </si>
+  <si>
+    <t>00:00:10</t>
+  </si>
+  <si>
+    <t>28/07/2026</t>
+  </si>
+  <si>
+    <t>00:00:11</t>
+  </si>
+  <si>
+    <t>28/07/2027</t>
+  </si>
+  <si>
+    <t>00:00:13</t>
+  </si>
+  <si>
+    <t>28/07/2029</t>
+  </si>
+  <si>
+    <t>00:00:14</t>
+  </si>
+  <si>
+    <t>28/07/2030</t>
+  </si>
+  <si>
+    <t>00:00:15</t>
+  </si>
+  <si>
+    <t>28/07/2031</t>
+  </si>
+  <si>
+    <t>00:00:16</t>
+  </si>
+  <si>
+    <t>28/07/2032</t>
+  </si>
+  <si>
+    <t>00:00:17</t>
+  </si>
+  <si>
+    <t>28/07/2033</t>
+  </si>
+  <si>
+    <t>00:00:18</t>
+  </si>
+  <si>
+    <t>28/07/2034</t>
+  </si>
+  <si>
+    <t>00:00:20</t>
+  </si>
+  <si>
+    <t>28/07/2036</t>
+  </si>
+  <si>
+    <t>00:00:21</t>
+  </si>
+  <si>
+    <t>28/07/2037</t>
+  </si>
+  <si>
+    <t>00:00:22</t>
+  </si>
+  <si>
+    <t>28/07/2038</t>
+  </si>
+  <si>
+    <t>00:00:23</t>
+  </si>
+  <si>
+    <t>28/07/2039</t>
+  </si>
+  <si>
+    <t>Usuario sem viagem - Cards</t>
+  </si>
+  <si>
+    <t>Usuario sem viagem - Brindes</t>
+  </si>
+  <si>
+    <t>Usuario sem viagem - Cupons</t>
+  </si>
+  <si>
+    <t>00:00:38</t>
+  </si>
+  <si>
+    <t>02/08/2021</t>
+  </si>
+  <si>
+    <t>Selecionar o brinde 1 (Agenda do carro).  Validar tela, textos e links deste brinde. Teste Botão Car10</t>
+  </si>
+  <si>
+    <t>00:01:49</t>
+  </si>
+  <si>
+    <t>Selecionar o brinde 2 (Check Up Automotivo). Validar tela, textos e links deste brinde. Teste Botão Car10</t>
+  </si>
+  <si>
+    <t>00:00:47</t>
+  </si>
+  <si>
+    <t>efetuar reteste para refatoração ou validação de defeito</t>
+  </si>
+  <si>
+    <t>é necessário alterar a massa de dados alterada antes da execução</t>
+  </si>
+  <si>
+    <t>03/08/2021</t>
+  </si>
+  <si>
+    <t>00:01:09</t>
+  </si>
+  <si>
+    <t>1.0.0.1662005</t>
+  </si>
+  <si>
+    <t>00:01:43</t>
+  </si>
+  <si>
+    <t>00:00:57</t>
+  </si>
+  <si>
     <t>00:01:11</t>
-  </si>
-  <si>
-    <t>00:01:43</t>
-  </si>
-  <si>
-    <t>30/07/2021</t>
-  </si>
-  <si>
-    <t>Captura tela dos cards</t>
-  </si>
-  <si>
-    <t>Captura tela dos cupons</t>
-  </si>
-  <si>
-    <t>CT63</t>
-  </si>
-  <si>
-    <t>CT64</t>
-  </si>
-  <si>
-    <t>CT65</t>
-  </si>
-  <si>
-    <t>00:00:06</t>
-  </si>
-  <si>
-    <t>28/07/2022</t>
-  </si>
-  <si>
-    <t>00:00:07</t>
-  </si>
-  <si>
-    <t>28/07/2023</t>
-  </si>
-  <si>
-    <t>00:00:08</t>
-  </si>
-  <si>
-    <t>28/07/2024</t>
-  </si>
-  <si>
-    <t>00:00:09</t>
-  </si>
-  <si>
-    <t>28/07/2025</t>
-  </si>
-  <si>
-    <t>00:00:10</t>
-  </si>
-  <si>
-    <t>28/07/2026</t>
-  </si>
-  <si>
-    <t>00:00:11</t>
-  </si>
-  <si>
-    <t>28/07/2027</t>
-  </si>
-  <si>
-    <t>00:00:13</t>
-  </si>
-  <si>
-    <t>28/07/2029</t>
-  </si>
-  <si>
-    <t>00:00:14</t>
-  </si>
-  <si>
-    <t>28/07/2030</t>
-  </si>
-  <si>
-    <t>00:00:15</t>
-  </si>
-  <si>
-    <t>28/07/2031</t>
-  </si>
-  <si>
-    <t>00:00:16</t>
-  </si>
-  <si>
-    <t>28/07/2032</t>
-  </si>
-  <si>
-    <t>00:00:17</t>
-  </si>
-  <si>
-    <t>28/07/2033</t>
-  </si>
-  <si>
-    <t>00:00:18</t>
-  </si>
-  <si>
-    <t>28/07/2034</t>
-  </si>
-  <si>
-    <t>00:00:20</t>
-  </si>
-  <si>
-    <t>28/07/2036</t>
-  </si>
-  <si>
-    <t>00:00:21</t>
-  </si>
-  <si>
-    <t>28/07/2037</t>
-  </si>
-  <si>
-    <t>00:00:22</t>
-  </si>
-  <si>
-    <t>28/07/2038</t>
-  </si>
-  <si>
-    <t>00:00:23</t>
-  </si>
-  <si>
-    <t>28/07/2039</t>
-  </si>
-  <si>
-    <t>Usuario sem viagem - Cards</t>
-  </si>
-  <si>
-    <t>Usuario sem viagem - Brindes</t>
-  </si>
-  <si>
-    <t>Usuario sem viagem - Cupons</t>
-  </si>
-  <si>
-    <t>00:00:38</t>
-  </si>
-  <si>
-    <t>02/08/2021</t>
-  </si>
-  <si>
-    <t>00:01:30</t>
-  </si>
-  <si>
-    <t>00:01:13</t>
-  </si>
-  <si>
-    <t>Selecionar o brinde 1 (Agenda do carro).  Validar tela, textos e links deste brinde. Teste Botão Car10</t>
-  </si>
-  <si>
-    <t>00:01:49</t>
-  </si>
-  <si>
-    <t>Selecionar o brinde 2 (Check Up Automotivo). Validar tela, textos e links deste brinde. Teste Botão Car10</t>
-  </si>
-  <si>
-    <t>00:00:45</t>
-  </si>
-  <si>
-    <t>00:00:47</t>
   </si>
 </sst>
 </file>
@@ -1593,7 +1593,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1738,6 +1738,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -1809,7 +1815,7 @@
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2010,6 +2016,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -10765,7 +10773,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10821,7 +10829,7 @@
         <v>123</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>124</v>
@@ -10890,16 +10898,16 @@
         <v>16</v>
       </c>
       <c r="AC1" s="67" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD1" s="67" t="s">
         <v>204</v>
       </c>
-      <c r="AD1" s="67" t="s">
+      <c r="AE1" s="67" t="s">
         <v>205</v>
       </c>
-      <c r="AE1" s="67" t="s">
-        <v>206</v>
-      </c>
       <c r="AF1" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AG1" s="2" t="s">
         <v>170</v>
@@ -10907,7 +10915,7 @@
     </row>
     <row r="2" spans="1:33">
       <c r="A2" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B2" s="83" t="s">
         <v>21</v>
@@ -10925,13 +10933,13 @@
         <v>111</v>
       </c>
       <c r="G2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H2" t="s">
-        <v>365</v>
+        <v>413</v>
       </c>
       <c r="I2" t="s">
-        <v>296</v>
+        <v>410</v>
       </c>
       <c r="J2" t="s">
         <v>133</v>
@@ -10943,10 +10951,10 @@
         <v>129</v>
       </c>
       <c r="M2" s="76" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O2" s="7" t="s">
         <v>131</v>
@@ -10982,7 +10990,7 @@
         <v>131</v>
       </c>
       <c r="Z2" s="92" t="s">
-        <v>316</v>
+        <v>412</v>
       </c>
       <c r="AA2" s="10">
         <v>44096</v>
@@ -11008,13 +11016,13 @@
     </row>
     <row r="3" spans="1:33">
       <c r="A3" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B3" s="104" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="93" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D3" t="s">
         <v>128</v>
@@ -11026,13 +11034,13 @@
         <v>111</v>
       </c>
       <c r="G3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H3" t="s">
+        <v>411</v>
+      </c>
+      <c r="I3" t="s">
         <v>410</v>
-      </c>
-      <c r="I3" t="s">
-        <v>408</v>
       </c>
       <c r="J3" t="s">
         <v>133</v>
@@ -11044,10 +11052,10 @@
         <v>129</v>
       </c>
       <c r="M3" s="90" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O3" s="7" t="s">
         <v>131</v>
@@ -11109,13 +11117,13 @@
     </row>
     <row r="4" spans="1:33">
       <c r="A4" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B4" s="104" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C4" s="93" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D4" t="s">
         <v>128</v>
@@ -11127,13 +11135,13 @@
         <v>111</v>
       </c>
       <c r="G4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H4" t="s">
-        <v>364</v>
+        <v>411</v>
       </c>
       <c r="I4" t="s">
-        <v>366</v>
+        <v>410</v>
       </c>
       <c r="J4" t="s">
         <v>133</v>
@@ -11145,10 +11153,10 @@
         <v>129</v>
       </c>
       <c r="M4" s="73" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O4" s="7" t="s">
         <v>131</v>
@@ -11210,13 +11218,13 @@
     </row>
     <row r="5" spans="1:33">
       <c r="A5" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B5" s="104" t="s">
+        <v>357</v>
+      </c>
+      <c r="C5" s="93" t="s">
         <v>360</v>
-      </c>
-      <c r="C5" s="93" t="s">
-        <v>363</v>
       </c>
       <c r="D5" t="s">
         <v>128</v>
@@ -11228,13 +11236,13 @@
         <v>111</v>
       </c>
       <c r="G5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H5" t="s">
-        <v>409</v>
+        <v>283</v>
       </c>
       <c r="I5" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="J5" t="s">
         <v>133</v>
@@ -11245,11 +11253,11 @@
       <c r="L5" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="M5" s="76" t="s">
-        <v>234</v>
+      <c r="M5" s="62" t="s">
+        <v>233</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O5" s="7" t="s">
         <v>131</v>
@@ -11311,7 +11319,7 @@
     </row>
     <row r="6" spans="1:33">
       <c r="A6" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>186</v>
@@ -11326,16 +11334,16 @@
         <v>111</v>
       </c>
       <c r="F6" t="s">
-        <v>285</v>
+        <v>111</v>
       </c>
       <c r="G6" t="s">
         <v>232</v>
       </c>
       <c r="H6" t="s">
-        <v>284</v>
+        <v>414</v>
       </c>
       <c r="I6" t="s">
-        <v>276</v>
+        <v>410</v>
       </c>
       <c r="J6" t="s">
         <v>133</v>
@@ -11412,7 +11420,7 @@
     </row>
     <row r="7" spans="1:33">
       <c r="A7" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B7" s="70" t="s">
         <v>29</v>
@@ -11430,13 +11438,13 @@
         <v>111</v>
       </c>
       <c r="G7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H7" t="s">
         <v>284</v>
       </c>
       <c r="I7" t="s">
-        <v>276</v>
+        <v>410</v>
       </c>
       <c r="J7" t="s">
         <v>133</v>
@@ -11513,7 +11521,7 @@
     </row>
     <row r="8" spans="1:33">
       <c r="A8" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B8" s="70" t="s">
         <v>31</v>
@@ -11528,16 +11536,16 @@
         <v>111</v>
       </c>
       <c r="F8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J8" t="s">
         <v>133</v>
@@ -11562,10 +11570,10 @@
       </c>
       <c r="Q8" s="8"/>
       <c r="R8" s="86" t="s">
+        <v>281</v>
+      </c>
+      <c r="S8" s="6" t="s">
         <v>282</v>
-      </c>
-      <c r="S8" s="6" t="s">
-        <v>283</v>
       </c>
       <c r="T8" t="s">
         <v>4</v>
@@ -11612,7 +11620,7 @@
     </row>
     <row r="9" spans="1:33">
       <c r="A9" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9" s="82" t="s">
         <v>31</v>
@@ -11630,13 +11638,13 @@
         <v>148</v>
       </c>
       <c r="G9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I9" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J9" t="s">
         <v>133</v>
@@ -11664,7 +11672,7 @@
         <v>3</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T9" t="s">
         <v>4</v>
@@ -11711,10 +11719,10 @@
     </row>
     <row r="10" spans="1:33">
       <c r="A10" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B10" s="82" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C10" s="74" t="s">
         <v>20</v>
@@ -11723,19 +11731,19 @@
         <v>128</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J10" t="s">
         <v>133</v>
@@ -11760,10 +11768,10 @@
       </c>
       <c r="Q10" s="8"/>
       <c r="R10" s="62" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S10" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T10" s="68" t="s">
         <v>4</v>
@@ -11810,7 +11818,7 @@
     </row>
     <row r="11" spans="1:33">
       <c r="A11" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>33</v>
@@ -11828,13 +11836,13 @@
         <v>111</v>
       </c>
       <c r="G11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J11" t="s">
         <v>133</v>
@@ -11846,10 +11854,10 @@
         <v>129</v>
       </c>
       <c r="M11" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N11" s="77" t="s">
         <v>252</v>
-      </c>
-      <c r="N11" s="77" t="s">
-        <v>253</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>131</v>
@@ -11911,7 +11919,7 @@
     </row>
     <row r="12" spans="1:33">
       <c r="A12" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>184</v>
@@ -11929,13 +11937,13 @@
         <v>111</v>
       </c>
       <c r="G12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H12" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J12" t="s">
         <v>133</v>
@@ -11947,10 +11955,10 @@
         <v>129</v>
       </c>
       <c r="M12" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N12" s="77" t="s">
         <v>252</v>
-      </c>
-      <c r="N12" s="77" t="s">
-        <v>253</v>
       </c>
       <c r="O12" s="7" t="s">
         <v>131</v>
@@ -12030,13 +12038,13 @@
         <v>111</v>
       </c>
       <c r="G13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I13" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J13" t="s">
         <v>133</v>
@@ -12048,10 +12056,10 @@
         <v>129</v>
       </c>
       <c r="M13" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N13" s="77" t="s">
         <v>252</v>
-      </c>
-      <c r="N13" s="77" t="s">
-        <v>253</v>
       </c>
       <c r="O13" s="7" t="s">
         <v>131</v>
@@ -12131,13 +12139,13 @@
         <v>111</v>
       </c>
       <c r="G14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J14" t="s">
         <v>133</v>
@@ -12149,10 +12157,10 @@
         <v>129</v>
       </c>
       <c r="M14" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N14" s="77" t="s">
         <v>252</v>
-      </c>
-      <c r="N14" s="77" t="s">
-        <v>253</v>
       </c>
       <c r="O14" s="7" t="s">
         <v>131</v>
@@ -12214,7 +12222,7 @@
     </row>
     <row r="15" spans="1:33">
       <c r="A15" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>138</v>
@@ -12232,13 +12240,13 @@
         <v>111</v>
       </c>
       <c r="G15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H15" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J15" t="s">
         <v>133</v>
@@ -12250,10 +12258,10 @@
         <v>128</v>
       </c>
       <c r="M15" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N15" s="77" t="s">
         <v>252</v>
-      </c>
-      <c r="N15" s="77" t="s">
-        <v>253</v>
       </c>
       <c r="O15" s="7" t="s">
         <v>131</v>
@@ -12315,13 +12323,13 @@
     </row>
     <row r="16" spans="1:33">
       <c r="A16" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>99</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D16" t="s">
         <v>128</v>
@@ -12333,13 +12341,13 @@
         <v>111</v>
       </c>
       <c r="G16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H16" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I16" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J16" t="s">
         <v>133</v>
@@ -12351,10 +12359,10 @@
         <v>129</v>
       </c>
       <c r="M16" s="76" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O16" s="7" t="s">
         <v>131</v>
@@ -12422,7 +12430,7 @@
         <v>42</v>
       </c>
       <c r="C17" s="74" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="D17" t="s">
         <v>128</v>
@@ -12434,13 +12442,13 @@
         <v>111</v>
       </c>
       <c r="G17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H17" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I17" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="J17" t="s">
         <v>133</v>
@@ -12452,10 +12460,10 @@
         <v>129</v>
       </c>
       <c r="M17" s="90" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="N17" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O17" s="7" t="s">
         <v>131</v>
@@ -12523,7 +12531,7 @@
         <v>43</v>
       </c>
       <c r="C18" s="74" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="D18" t="s">
         <v>128</v>
@@ -12535,13 +12543,13 @@
         <v>111</v>
       </c>
       <c r="G18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H18" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="I18" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="J18" t="s">
         <v>133</v>
@@ -12553,10 +12561,10 @@
         <v>129</v>
       </c>
       <c r="M18" s="109" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="N18" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O18" s="7" t="s">
         <v>131</v>
@@ -12623,7 +12631,7 @@
       <c r="B19" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="78" t="s">
+      <c r="C19" s="74" t="s">
         <v>101</v>
       </c>
       <c r="D19" t="s">
@@ -12636,13 +12644,13 @@
         <v>111</v>
       </c>
       <c r="G19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H19" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="I19" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="J19" t="s">
         <v>133</v>
@@ -12654,10 +12662,10 @@
         <v>129</v>
       </c>
       <c r="M19" s="109" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="N19" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O19" s="7" t="s">
         <v>131</v>
@@ -12719,31 +12727,31 @@
     </row>
     <row r="20" spans="1:33">
       <c r="A20" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="B20" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="B20" s="110" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="94" t="s">
         <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>111</v>
       </c>
       <c r="F20" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H20" t="s">
-        <v>304</v>
+        <v>415</v>
       </c>
       <c r="I20" t="s">
-        <v>296</v>
+        <v>410</v>
       </c>
       <c r="J20" t="s">
         <v>133</v>
@@ -12755,10 +12763,10 @@
         <v>129</v>
       </c>
       <c r="M20" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N20" s="77" t="s">
         <v>252</v>
-      </c>
-      <c r="N20" s="77" t="s">
-        <v>253</v>
       </c>
       <c r="O20" s="7" t="s">
         <v>131</v>
@@ -12820,13 +12828,13 @@
     </row>
     <row r="21" spans="1:33">
       <c r="A21" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>50</v>
       </c>
       <c r="C21" s="97" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D21" t="s">
         <v>128</v>
@@ -12838,13 +12846,13 @@
         <v>111</v>
       </c>
       <c r="G21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H21" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I21" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J21" t="s">
         <v>133</v>
@@ -12856,10 +12864,10 @@
         <v>129</v>
       </c>
       <c r="M21" s="90" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="N21" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O21" s="7" t="s">
         <v>131</v>
@@ -12921,7 +12929,7 @@
     </row>
     <row r="22" spans="1:33">
       <c r="A22" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>51</v>
@@ -12939,13 +12947,13 @@
         <v>111</v>
       </c>
       <c r="G22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I22" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J22" t="s">
         <v>133</v>
@@ -12957,10 +12965,10 @@
         <v>129</v>
       </c>
       <c r="M22" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N22" s="77" t="s">
         <v>252</v>
-      </c>
-      <c r="N22" s="77" t="s">
-        <v>253</v>
       </c>
       <c r="O22" s="7" t="s">
         <v>131</v>
@@ -13040,13 +13048,13 @@
         <v>111</v>
       </c>
       <c r="G23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I23" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J23" t="s">
         <v>133</v>
@@ -13058,10 +13066,10 @@
         <v>129</v>
       </c>
       <c r="M23" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N23" s="77" t="s">
         <v>252</v>
-      </c>
-      <c r="N23" s="77" t="s">
-        <v>253</v>
       </c>
       <c r="O23" s="7" t="s">
         <v>131</v>
@@ -13141,13 +13149,13 @@
         <v>111</v>
       </c>
       <c r="G24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I24" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J24" t="s">
         <v>133</v>
@@ -13159,10 +13167,10 @@
         <v>129</v>
       </c>
       <c r="M24" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N24" s="77" t="s">
         <v>252</v>
-      </c>
-      <c r="N24" s="77" t="s">
-        <v>253</v>
       </c>
       <c r="O24" s="7" t="s">
         <v>131</v>
@@ -13227,10 +13235,10 @@
         <v>45</v>
       </c>
       <c r="B25" s="91" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C25" s="89" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D25" t="s">
         <v>128</v>
@@ -13239,16 +13247,16 @@
         <v>111</v>
       </c>
       <c r="F25" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H25" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I25" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J25" t="s">
         <v>133</v>
@@ -13260,10 +13268,10 @@
         <v>129</v>
       </c>
       <c r="M25" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N25" s="77" t="s">
         <v>252</v>
-      </c>
-      <c r="N25" s="77" t="s">
-        <v>253</v>
       </c>
       <c r="O25" s="7" t="s">
         <v>131</v>
@@ -13328,10 +13336,10 @@
         <v>46</v>
       </c>
       <c r="B26" s="91" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C26" s="89" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D26" t="s">
         <v>128</v>
@@ -13340,16 +13348,16 @@
         <v>111</v>
       </c>
       <c r="F26" t="s">
+        <v>253</v>
+      </c>
+      <c r="G26" t="s">
+        <v>231</v>
+      </c>
+      <c r="H26" t="s">
         <v>254</v>
       </c>
-      <c r="G26" t="s">
-        <v>232</v>
-      </c>
-      <c r="H26" t="s">
-        <v>255</v>
-      </c>
       <c r="I26" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J26" t="s">
         <v>133</v>
@@ -13361,10 +13369,10 @@
         <v>129</v>
       </c>
       <c r="M26" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N26" s="77" t="s">
         <v>252</v>
-      </c>
-      <c r="N26" s="77" t="s">
-        <v>253</v>
       </c>
       <c r="O26" s="7" t="s">
         <v>131</v>
@@ -13429,7 +13437,7 @@
         <v>102</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C27" s="93" t="s">
         <v>109</v>
@@ -13444,13 +13452,13 @@
         <v>111</v>
       </c>
       <c r="G27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H27" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I27" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J27" t="s">
         <v>133</v>
@@ -13530,7 +13538,7 @@
         <v>103</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C28" s="74" t="s">
         <v>110</v>
@@ -13545,13 +13553,13 @@
         <v>111</v>
       </c>
       <c r="G28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H28" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I28" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J28" t="s">
         <v>133</v>
@@ -13563,10 +13571,10 @@
         <v>129</v>
       </c>
       <c r="M28" s="63" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O28" s="7" t="s">
         <v>131</v>
@@ -13631,28 +13639,28 @@
         <v>104</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C29" s="74" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D29" t="s">
         <v>128</v>
       </c>
       <c r="E29" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F29" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H29" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J29" t="s">
         <v>133</v>
@@ -13664,11 +13672,11 @@
         <v>129</v>
       </c>
       <c r="M29" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N29" s="77" t="s">
         <v>252</v>
       </c>
-      <c r="N29" s="77" t="s">
-        <v>253</v>
-      </c>
       <c r="O29" s="7" t="s">
         <v>131</v>
       </c>
@@ -13712,13 +13720,13 @@
         <v>131</v>
       </c>
       <c r="AC29" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="AD29" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="AE29" s="7" t="s">
         <v>277</v>
-      </c>
-      <c r="AD29" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="AE29" s="7" t="s">
-        <v>278</v>
       </c>
       <c r="AF29" s="7" t="s">
         <v>131</v>
@@ -13735,7 +13743,7 @@
         <v>113</v>
       </c>
       <c r="C30" s="74" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D30" t="s">
         <v>128</v>
@@ -13747,13 +13755,13 @@
         <v>111</v>
       </c>
       <c r="G30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H30" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I30" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J30" t="s">
         <v>133</v>
@@ -13765,10 +13773,10 @@
         <v>129</v>
       </c>
       <c r="M30" s="79" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N30" s="80" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O30" s="7" t="s">
         <v>131</v>
@@ -13833,10 +13841,10 @@
         <v>106</v>
       </c>
       <c r="B31" s="91" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C31" s="75" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D31" t="s">
         <v>128</v>
@@ -13873,13 +13881,13 @@
     </row>
     <row r="32" spans="1:33">
       <c r="A32" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B32" s="91" t="s">
         <v>115</v>
       </c>
       <c r="C32" s="74" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D32" t="s">
         <v>128</v>
@@ -13891,13 +13899,13 @@
         <v>111</v>
       </c>
       <c r="G32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H32" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I32" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J32" t="s">
         <v>133</v>
@@ -13909,10 +13917,10 @@
         <v>129</v>
       </c>
       <c r="M32" s="76" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O32" s="7" t="s">
         <v>131</v>
@@ -13936,7 +13944,7 @@
         <v>131</v>
       </c>
       <c r="W32" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="X32" s="7" t="s">
         <v>131</v>
@@ -13971,13 +13979,13 @@
     </row>
     <row r="33" spans="1:33">
       <c r="A33" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B33" s="91" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C33" s="74" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D33" t="s">
         <v>128</v>
@@ -13989,13 +13997,13 @@
         <v>111</v>
       </c>
       <c r="G33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H33" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I33" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J33" t="s">
         <v>133</v>
@@ -14007,10 +14015,10 @@
         <v>129</v>
       </c>
       <c r="M33" s="76" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N33" s="84" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O33" s="7" t="s">
         <v>131</v>
@@ -14034,7 +14042,7 @@
         <v>131</v>
       </c>
       <c r="W33" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="X33" s="7" t="s">
         <v>131</v>
@@ -14069,7 +14077,7 @@
     </row>
     <row r="34" spans="1:33">
       <c r="A34" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>27</v>
@@ -14087,13 +14095,13 @@
         <v>111</v>
       </c>
       <c r="G34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H34" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I34" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J34" t="s">
         <v>133</v>
@@ -14105,10 +14113,10 @@
         <v>129</v>
       </c>
       <c r="M34" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N34" s="77" t="s">
         <v>252</v>
-      </c>
-      <c r="N34" s="77" t="s">
-        <v>253</v>
       </c>
       <c r="O34" s="7" t="s">
         <v>131</v>
@@ -14176,7 +14184,7 @@
         <v>48</v>
       </c>
       <c r="C35" s="100" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D35" t="s">
         <v>128</v>
@@ -14185,16 +14193,16 @@
         <v>111</v>
       </c>
       <c r="F35" t="s">
+        <v>241</v>
+      </c>
+      <c r="G35" t="s">
+        <v>231</v>
+      </c>
+      <c r="H35" t="s">
         <v>242</v>
       </c>
-      <c r="G35" t="s">
-        <v>232</v>
-      </c>
-      <c r="H35" t="s">
-        <v>243</v>
-      </c>
       <c r="I35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J35" t="s">
         <v>133</v>
@@ -14207,7 +14215,7 @@
       </c>
       <c r="M35" s="63"/>
       <c r="N35" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O35" s="7" t="s">
         <v>131</v>
@@ -14269,13 +14277,13 @@
     </row>
     <row r="36" spans="1:33">
       <c r="A36" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B36" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="C36" s="74" t="s">
         <v>208</v>
-      </c>
-      <c r="C36" s="74" t="s">
-        <v>209</v>
       </c>
       <c r="D36" t="s">
         <v>128</v>
@@ -14287,13 +14295,13 @@
         <v>111</v>
       </c>
       <c r="G36" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H36" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I36" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J36" t="s">
         <v>133</v>
@@ -14305,10 +14313,10 @@
         <v>129</v>
       </c>
       <c r="M36" s="90" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="N36" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O36" s="7" t="s">
         <v>131</v>
@@ -14370,7 +14378,7 @@
     </row>
     <row r="37" spans="1:33">
       <c r="A37" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>119</v>
@@ -14388,13 +14396,13 @@
         <v>111</v>
       </c>
       <c r="G37" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H37" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="I37" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J37" s="85" t="s">
         <v>49</v>
@@ -14412,7 +14420,7 @@
         <v>131</v>
       </c>
       <c r="O37" s="79" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="P37" s="7" t="s">
         <v>131</v>
@@ -14424,7 +14432,7 @@
         <v>3</v>
       </c>
       <c r="S37" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T37" s="85" t="s">
         <v>4</v>
@@ -14471,7 +14479,7 @@
     </row>
     <row r="38" spans="1:33">
       <c r="A38" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B38" s="91" t="s">
         <v>56</v>
@@ -14489,13 +14497,13 @@
         <v>111</v>
       </c>
       <c r="G38" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H38" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I38" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J38" t="s">
         <v>133</v>
@@ -14507,11 +14515,11 @@
         <v>129</v>
       </c>
       <c r="M38" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N38" s="77" t="s">
         <v>252</v>
       </c>
-      <c r="N38" s="77" t="s">
-        <v>253</v>
-      </c>
       <c r="O38" s="7" t="s">
         <v>131</v>
       </c>
@@ -14552,7 +14560,7 @@
         <v>131</v>
       </c>
       <c r="AB38" s="73" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="AC38" s="7" t="s">
         <v>131</v>
@@ -14572,7 +14580,7 @@
     </row>
     <row r="39" spans="1:33">
       <c r="A39" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B39" s="101" t="s">
         <v>58</v>
@@ -14587,16 +14595,16 @@
         <v>111</v>
       </c>
       <c r="F39" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G39" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H39" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I39" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J39" t="s">
         <v>133</v>
@@ -14608,10 +14616,10 @@
         <v>129</v>
       </c>
       <c r="M39" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N39" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O39" s="7" t="s">
         <v>131</v>
@@ -14688,16 +14696,16 @@
         <v>111</v>
       </c>
       <c r="F40" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G40" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H40" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J40" t="s">
         <v>133</v>
@@ -14709,10 +14717,10 @@
         <v>129</v>
       </c>
       <c r="M40" s="76" t="s">
+        <v>251</v>
+      </c>
+      <c r="N40" s="77" t="s">
         <v>252</v>
-      </c>
-      <c r="N40" s="77" t="s">
-        <v>253</v>
       </c>
       <c r="O40" s="7" t="s">
         <v>131</v>
@@ -14792,13 +14800,13 @@
         <v>111</v>
       </c>
       <c r="G41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H41" t="s">
+        <v>238</v>
+      </c>
+      <c r="I41" t="s">
         <v>239</v>
-      </c>
-      <c r="I41" t="s">
-        <v>240</v>
       </c>
       <c r="J41" t="s">
         <v>49</v>
@@ -14867,10 +14875,10 @@
         <v>131</v>
       </c>
       <c r="AF41" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AG41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="42" spans="1:33">
@@ -14881,25 +14889,25 @@
         <v>31</v>
       </c>
       <c r="C42" s="74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D42" t="s">
         <v>128</v>
       </c>
       <c r="E42" s="65" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F42" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G42" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H42" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I42" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J42" t="s">
         <v>133</v>
@@ -14927,10 +14935,10 @@
         <v>3</v>
       </c>
       <c r="S42" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T42" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="U42" t="s">
         <v>5</v>
@@ -14974,13 +14982,13 @@
     </row>
     <row r="43" spans="1:33">
       <c r="A43" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B43" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C43" s="74" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D43" t="s">
         <v>128</v>
@@ -14992,13 +15000,13 @@
         <v>172</v>
       </c>
       <c r="G43" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I43" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J43" t="s">
         <v>133</v>
@@ -15073,31 +15081,31 @@
     </row>
     <row r="44" spans="1:33">
       <c r="A44" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C44" s="74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D44" t="s">
         <v>128</v>
       </c>
       <c r="E44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H44" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="I44" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J44" t="s">
         <v>133</v>
@@ -15122,10 +15130,10 @@
       </c>
       <c r="Q44" s="30"/>
       <c r="R44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="S44" s="77" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T44" t="s">
         <v>4</v>
@@ -15172,13 +15180,13 @@
     </row>
     <row r="47" spans="1:33">
       <c r="A47" s="107" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B47" s="105" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C47" s="105" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D47" t="s">
         <v>128</v>
@@ -15190,13 +15198,13 @@
         <v>111</v>
       </c>
       <c r="G47" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H47" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I47" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="J47" t="s">
         <v>133</v>
@@ -15208,10 +15216,10 @@
         <v>129</v>
       </c>
       <c r="M47" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N47" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O47" s="7" t="s">
         <v>131</v>
@@ -15273,13 +15281,13 @@
     </row>
     <row r="48" spans="1:33">
       <c r="A48" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B48" s="105" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C48" s="105" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D48" t="s">
         <v>128</v>
@@ -15288,16 +15296,16 @@
         <v>111</v>
       </c>
       <c r="F48" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H48" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I48" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J48" t="s">
         <v>133</v>
@@ -15309,10 +15317,10 @@
         <v>129</v>
       </c>
       <c r="M48" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N48" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O48" s="7" t="s">
         <v>131</v>
@@ -15374,13 +15382,13 @@
     </row>
     <row r="49" spans="1:33">
       <c r="A49" s="14" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B49" s="105" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C49" s="105" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D49" t="s">
         <v>128</v>
@@ -15389,16 +15397,16 @@
         <v>111</v>
       </c>
       <c r="F49" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G49" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H49" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="I49" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="J49" t="s">
         <v>133</v>
@@ -15410,10 +15418,10 @@
         <v>129</v>
       </c>
       <c r="M49" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N49" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O49" s="7" t="s">
         <v>131</v>
@@ -15475,13 +15483,13 @@
     </row>
     <row r="50" spans="1:33">
       <c r="A50" s="14" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B50" s="105" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C50" s="105" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D50" t="s">
         <v>128</v>
@@ -15490,16 +15498,16 @@
         <v>111</v>
       </c>
       <c r="F50" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H50" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="I50" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="J50" t="s">
         <v>133</v>
@@ -15511,10 +15519,10 @@
         <v>129</v>
       </c>
       <c r="M50" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N50" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O50" s="7" t="s">
         <v>131</v>
@@ -15579,10 +15587,10 @@
         <v>60</v>
       </c>
       <c r="B51" s="105" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C51" s="105" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D51" t="s">
         <v>128</v>
@@ -15591,16 +15599,16 @@
         <v>111</v>
       </c>
       <c r="F51" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G51" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H51" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="I51" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="J51" t="s">
         <v>133</v>
@@ -15612,10 +15620,10 @@
         <v>129</v>
       </c>
       <c r="M51" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N51" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O51" s="7" t="s">
         <v>131</v>
@@ -15680,10 +15688,10 @@
         <v>61</v>
       </c>
       <c r="B52" s="105" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C52" s="105" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D52" t="s">
         <v>128</v>
@@ -15692,16 +15700,16 @@
         <v>111</v>
       </c>
       <c r="F52" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G52" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H52" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="I52" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="J52" t="s">
         <v>133</v>
@@ -15713,10 +15721,10 @@
         <v>129</v>
       </c>
       <c r="M52" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N52" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O52" s="7" t="s">
         <v>131</v>
@@ -15778,13 +15786,13 @@
     </row>
     <row r="53" spans="1:33">
       <c r="A53" s="14" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B53" s="105" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C53" s="105" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D53" t="s">
         <v>128</v>
@@ -15793,16 +15801,16 @@
         <v>111</v>
       </c>
       <c r="F53" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G53" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H53" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="I53" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="J53" t="s">
         <v>133</v>
@@ -15814,10 +15822,10 @@
         <v>129</v>
       </c>
       <c r="M53" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N53" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O53" s="7" t="s">
         <v>131</v>
@@ -15879,13 +15887,13 @@
     </row>
     <row r="54" spans="1:33">
       <c r="A54" s="14" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B54" s="105" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C54" s="105" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D54" t="s">
         <v>128</v>
@@ -15894,16 +15902,16 @@
         <v>111</v>
       </c>
       <c r="F54" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G54" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H54" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I54" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="J54" t="s">
         <v>133</v>
@@ -15915,10 +15923,10 @@
         <v>129</v>
       </c>
       <c r="M54" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N54" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O54" s="7" t="s">
         <v>131</v>
@@ -15980,13 +15988,13 @@
     </row>
     <row r="55" spans="1:33">
       <c r="A55" s="107" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B55" s="106" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C55" s="106" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D55" t="s">
         <v>128</v>
@@ -15998,13 +16006,13 @@
         <v>111</v>
       </c>
       <c r="G55" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H55" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I55" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="J55" t="s">
         <v>133</v>
@@ -16016,10 +16024,10 @@
         <v>129</v>
       </c>
       <c r="M55" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N55" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O55" s="7" t="s">
         <v>131</v>
@@ -16081,13 +16089,13 @@
     </row>
     <row r="56" spans="1:33">
       <c r="A56" s="14" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B56" s="106" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C56" s="106" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D56" t="s">
         <v>128</v>
@@ -16096,16 +16104,16 @@
         <v>111</v>
       </c>
       <c r="F56" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G56" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H56" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="I56" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="J56" t="s">
         <v>133</v>
@@ -16117,10 +16125,10 @@
         <v>129</v>
       </c>
       <c r="M56" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N56" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O56" s="7" t="s">
         <v>131</v>
@@ -16182,13 +16190,13 @@
     </row>
     <row r="57" spans="1:33">
       <c r="A57" s="14" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B57" s="106" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C57" s="106" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D57" t="s">
         <v>128</v>
@@ -16197,16 +16205,16 @@
         <v>111</v>
       </c>
       <c r="F57" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G57" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H57" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="I57" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="J57" t="s">
         <v>133</v>
@@ -16218,10 +16226,10 @@
         <v>129</v>
       </c>
       <c r="M57" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N57" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O57" s="7" t="s">
         <v>131</v>
@@ -16283,13 +16291,13 @@
     </row>
     <row r="58" spans="1:33">
       <c r="A58" s="108" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B58" s="106" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C58" s="106" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D58" t="s">
         <v>128</v>
@@ -16298,16 +16306,16 @@
         <v>111</v>
       </c>
       <c r="F58" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H58" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I58" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="J58" t="s">
         <v>133</v>
@@ -16319,10 +16327,10 @@
         <v>129</v>
       </c>
       <c r="M58" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N58" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O58" s="7" t="s">
         <v>131</v>
@@ -16384,13 +16392,13 @@
     </row>
     <row r="59" spans="1:33">
       <c r="A59" s="14" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B59" s="106" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C59" s="106" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D59" t="s">
         <v>128</v>
@@ -16399,16 +16407,16 @@
         <v>111</v>
       </c>
       <c r="F59" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G59" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H59" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="I59" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="J59" t="s">
         <v>133</v>
@@ -16420,10 +16428,10 @@
         <v>129</v>
       </c>
       <c r="M59" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N59" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O59" s="7" t="s">
         <v>131</v>
@@ -16485,13 +16493,13 @@
     </row>
     <row r="60" spans="1:33">
       <c r="A60" s="14" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B60" s="106" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C60" s="106" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D60" t="s">
         <v>128</v>
@@ -16500,16 +16508,16 @@
         <v>111</v>
       </c>
       <c r="F60" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G60" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H60" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="I60" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="J60" t="s">
         <v>133</v>
@@ -16521,10 +16529,10 @@
         <v>129</v>
       </c>
       <c r="M60" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N60" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O60" s="7" t="s">
         <v>131</v>
@@ -16586,13 +16594,13 @@
     </row>
     <row r="61" spans="1:33">
       <c r="A61" s="14" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B61" s="106" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C61" s="106" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D61" t="s">
         <v>128</v>
@@ -16601,16 +16609,16 @@
         <v>111</v>
       </c>
       <c r="F61" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G61" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H61" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I61" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="J61" t="s">
         <v>133</v>
@@ -16622,10 +16630,10 @@
         <v>129</v>
       </c>
       <c r="M61" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N61" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O61" s="7" t="s">
         <v>131</v>
@@ -16687,13 +16695,13 @@
     </row>
     <row r="62" spans="1:33">
       <c r="A62" s="107" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B62" s="105" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="C62" s="105" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="D62" t="s">
         <v>128</v>
@@ -16705,13 +16713,13 @@
         <v>111</v>
       </c>
       <c r="G62" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H62" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I62" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="J62" t="s">
         <v>133</v>
@@ -16723,10 +16731,10 @@
         <v>129</v>
       </c>
       <c r="M62" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N62" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O62" s="7" t="s">
         <v>131</v>
@@ -16788,13 +16796,13 @@
     </row>
     <row r="63" spans="1:33">
       <c r="A63" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B63" s="105" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C63" s="105" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D63" t="s">
         <v>128</v>
@@ -16803,16 +16811,16 @@
         <v>111</v>
       </c>
       <c r="F63" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G63" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H63" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="I63" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="J63" t="s">
         <v>133</v>
@@ -16824,10 +16832,10 @@
         <v>129</v>
       </c>
       <c r="M63" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N63" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O63" s="7" t="s">
         <v>131</v>
@@ -16889,13 +16897,13 @@
     </row>
     <row r="64" spans="1:33">
       <c r="A64" s="14" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B64" s="105" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C64" s="105" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D64" t="s">
         <v>128</v>
@@ -16904,16 +16912,16 @@
         <v>111</v>
       </c>
       <c r="F64" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G64" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H64" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="I64" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="J64" t="s">
         <v>133</v>
@@ -16925,10 +16933,10 @@
         <v>129</v>
       </c>
       <c r="M64" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N64" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O64" s="7" t="s">
         <v>131</v>
@@ -16990,13 +16998,13 @@
     </row>
     <row r="65" spans="1:35">
       <c r="A65" s="14" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B65" s="105" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C65" s="105" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D65" t="s">
         <v>128</v>
@@ -17005,16 +17013,16 @@
         <v>111</v>
       </c>
       <c r="F65" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H65" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="I65" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="J65" t="s">
         <v>133</v>
@@ -17026,10 +17034,10 @@
         <v>129</v>
       </c>
       <c r="M65" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N65" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O65" s="7" t="s">
         <v>131</v>
@@ -17091,13 +17099,13 @@
     </row>
     <row r="66" spans="1:35">
       <c r="A66" s="14" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B66" s="105" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C66" s="105" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D66" t="s">
         <v>128</v>
@@ -17106,16 +17114,16 @@
         <v>111</v>
       </c>
       <c r="F66" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G66" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H66" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="I66" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="J66" t="s">
         <v>133</v>
@@ -17127,10 +17135,10 @@
         <v>129</v>
       </c>
       <c r="M66" s="88" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N66" s="77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O66" s="7" t="s">
         <v>131</v>
@@ -17224,39 +17232,45 @@
       <c r="AF67" s="7"/>
       <c r="AG67" s="7"/>
     </row>
+    <row r="68" spans="1:35">
+      <c r="B68" s="111"/>
+      <c r="C68" s="110" t="s">
+        <v>408</v>
+      </c>
+    </row>
     <row r="69" spans="1:35">
-      <c r="B69" s="98" t="s">
-        <v>188</v>
-      </c>
-      <c r="C69" s="75"/>
+      <c r="B69" s="98"/>
+      <c r="C69" s="98" t="s">
+        <v>409</v>
+      </c>
       <c r="AI69" s="40"/>
     </row>
     <row r="70" spans="1:35">
       <c r="B70" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C70" s="73" t="s">
         <v>244</v>
-      </c>
-      <c r="C70" s="73" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="71" spans="1:35">
       <c r="B71" s="73" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C71" s="29" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="72" spans="1:35">
       <c r="B72" s="87" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C72" s="29" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
-    <row r="74" spans="1:35">
-      <c r="B74" s="63"/>
+    <row r="77" spans="1:35">
+      <c r="C77" s="88"/>
     </row>
     <row r="82" spans="2:2" ht="18">
       <c r="B82" s="71"/>
@@ -20907,10 +20921,11 @@
     <hyperlink ref="M17" r:id="rId8"/>
     <hyperlink ref="M18" r:id="rId9"/>
     <hyperlink ref="M19" r:id="rId10"/>
+    <hyperlink ref="M5" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
-  <legacyDrawing r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <legacyDrawing r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -20962,11 +20977,11 @@
       <c r="E2" s="41"/>
       <c r="F2" s="41"/>
       <c r="G2" s="41"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
       <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="7.5" customHeight="1">
@@ -20986,21 +21001,21 @@
     </row>
     <row r="4" spans="1:13" s="61" customFormat="1" ht="26.25" customHeight="1">
       <c r="A4" s="60"/>
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="114" t="s">
         <v>161</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="112" t="s">
+      <c r="H4" s="114" t="s">
         <v>162</v>
       </c>
-      <c r="I4" s="112"/>
-      <c r="J4" s="112"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="112"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="114"/>
       <c r="M4" s="60"/>
     </row>
     <row r="5" spans="1:13" ht="15">
@@ -21020,15 +21035,15 @@
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1">
       <c r="A6" s="44"/>
-      <c r="B6" s="114" t="s">
+      <c r="B6" s="116" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
       <c r="F6" s="51">
         <f>(J11+K11)/I11</f>
-        <v>0.97560975609756095</v>
+        <v>1</v>
       </c>
       <c r="G6" s="44"/>
       <c r="H6" s="38"/>
@@ -21048,10 +21063,10 @@
     </row>
     <row r="7" spans="1:13" ht="25.5">
       <c r="A7" s="44"/>
-      <c r="B7" s="114"/>
-      <c r="C7" s="113"/>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="115"/>
+      <c r="D7" s="115"/>
+      <c r="E7" s="115"/>
       <c r="F7" s="52" t="s">
         <v>176</v>
       </c>
@@ -21065,7 +21080,7 @@
       </c>
       <c r="J7" s="39">
         <f>COUNTIFS(Testes!G3:G45,"Passed",Testes!J3:J45,"Android")</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K7" s="39">
         <f>COUNTIFS(Testes!G3:G45,"Failed",Testes!J3:J45,"Android")</f>
@@ -21082,9 +21097,9 @@
         <f>COUNTIF(Testes!A3:A45,"&lt;&gt;"&amp;"")</f>
         <v>42</v>
       </c>
-      <c r="C8" s="113"/>
-      <c r="D8" s="113"/>
-      <c r="E8" s="113"/>
+      <c r="C8" s="115"/>
+      <c r="D8" s="115"/>
+      <c r="E8" s="115"/>
       <c r="F8" s="54"/>
       <c r="G8" s="44"/>
       <c r="H8" s="48" t="s">
@@ -21110,9 +21125,9 @@
     <row r="9" spans="1:13" ht="23.25">
       <c r="A9" s="44"/>
       <c r="B9" s="55"/>
-      <c r="C9" s="113"/>
-      <c r="D9" s="113"/>
-      <c r="E9" s="113"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
       <c r="F9" s="56">
         <f>SUM(Testes!H3:H45)</f>
         <v>0</v>
@@ -21143,17 +21158,17 @@
       <c r="B10" s="55"/>
       <c r="C10" s="39">
         <f>B8-(D10+E10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="39">
         <f>J11</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="39">
         <f>K11</f>
         <v>8</v>
       </c>
-      <c r="F10" s="110" t="s">
+      <c r="F10" s="112" t="s">
         <v>179</v>
       </c>
       <c r="G10" s="45"/>
@@ -21176,7 +21191,7 @@
       <c r="E11" s="57" t="s">
         <v>164</v>
       </c>
-      <c r="F11" s="110"/>
+      <c r="F11" s="112"/>
       <c r="G11" s="45"/>
       <c r="H11" s="39" t="s">
         <v>175</v>
@@ -21187,7 +21202,7 @@
       </c>
       <c r="J11" s="39">
         <f>SUM(J7:J9)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K11" s="39">
         <f>SUM(K7:K9)</f>
@@ -21469,7 +21484,7 @@
         <v>93</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -21487,7 +21502,7 @@
         <v>65</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>66</v>
@@ -21540,7 +21555,7 @@
         <v>131</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F2" s="30" t="s">
         <v>147</v>
@@ -21596,7 +21611,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>168</v>
@@ -21605,10 +21620,10 @@
         <v>167</v>
       </c>
       <c r="D3" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>217</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>218</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>147</v>
@@ -21617,7 +21632,7 @@
         <v>78</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I3" s="26" t="s">
         <v>79</v>
@@ -21846,30 +21861,30 @@
       <c r="D32" s="11"/>
     </row>
     <row r="33" spans="1:22">
-      <c r="A33" s="115" t="s">
+      <c r="A33" s="117" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="115"/>
-      <c r="C33" s="115"/>
-      <c r="D33" s="115"/>
-      <c r="E33" s="115"/>
-      <c r="F33" s="115"/>
-      <c r="G33" s="115"/>
-      <c r="H33" s="115"/>
-      <c r="I33" s="115"/>
-      <c r="J33" s="115"/>
-      <c r="K33" s="115"/>
-      <c r="L33" s="115"/>
-      <c r="M33" s="115"/>
-      <c r="N33" s="115"/>
-      <c r="O33" s="115"/>
-      <c r="P33" s="115"/>
-      <c r="Q33" s="115"/>
-      <c r="R33" s="115"/>
-      <c r="S33" s="115"/>
-      <c r="T33" s="115"/>
-      <c r="U33" s="115"/>
-      <c r="V33" s="115"/>
+      <c r="B33" s="117"/>
+      <c r="C33" s="117"/>
+      <c r="D33" s="117"/>
+      <c r="E33" s="117"/>
+      <c r="F33" s="117"/>
+      <c r="G33" s="117"/>
+      <c r="H33" s="117"/>
+      <c r="I33" s="117"/>
+      <c r="J33" s="117"/>
+      <c r="K33" s="117"/>
+      <c r="L33" s="117"/>
+      <c r="M33" s="117"/>
+      <c r="N33" s="117"/>
+      <c r="O33" s="117"/>
+      <c r="P33" s="117"/>
+      <c r="Q33" s="117"/>
+      <c r="R33" s="117"/>
+      <c r="S33" s="117"/>
+      <c r="T33" s="117"/>
+      <c r="U33" s="117"/>
+      <c r="V33" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
teste abrir manifestação ok, refatorado
</commit_message>
<xml_diff>
--- a/data/AutoVC.xlsx
+++ b/data/AutoVC.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2274" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2295" uniqueCount="419">
   <si>
     <t>Telefone</t>
   </si>
@@ -1013,349 +1013,358 @@
     <t>00:01:12</t>
   </si>
   <si>
+    <t>00:01:31</t>
+  </si>
+  <si>
+    <t>Falha ao concordar com os termos</t>
+  </si>
+  <si>
+    <t>Selecionar ranking geral.  Validar que ranking está vindo ordenado pelo score dos usuários. ( todos os testes de filtro, os filtros são aplicados mas não é feita validação de ordem de score)</t>
+  </si>
+  <si>
+    <t>00:00:54</t>
+  </si>
+  <si>
+    <t>00:00:48</t>
+  </si>
+  <si>
+    <t>Inicio esperado[Ínicio - 08:57 hs.] recebido[Ínicio - 18:56 hs.]</t>
+  </si>
+  <si>
+    <t>Chegada - 18:56 hs.</t>
+  </si>
+  <si>
+    <t>00:01:48</t>
+  </si>
+  <si>
+    <t>00:01:00</t>
+  </si>
+  <si>
+    <t>00:02:01</t>
+  </si>
+  <si>
+    <t>00:01:34</t>
+  </si>
+  <si>
+    <t>https://autovc.page.link/GcZk</t>
+  </si>
+  <si>
+    <t>00:00:35</t>
+  </si>
+  <si>
+    <t>00:01:16</t>
+  </si>
+  <si>
+    <t>00:01:24</t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Ordem dos cards</t>
+  </si>
+  <si>
+    <t>Validar que ao logar com um usuário novo, os cards virão na seguinte ordem: Iniciante / Direção / Amizade / Agenda do carro / Check up do carro / Smiles</t>
+  </si>
+  <si>
+    <t>CT46</t>
+  </si>
+  <si>
+    <t>CT47</t>
+  </si>
+  <si>
+    <t>CT48</t>
+  </si>
+  <si>
+    <t>CT49</t>
+  </si>
+  <si>
+    <t>CT52</t>
+  </si>
+  <si>
+    <t>CT53</t>
+  </si>
+  <si>
+    <t>CT54</t>
+  </si>
+  <si>
+    <t>CT55</t>
+  </si>
+  <si>
+    <t>CT56</t>
+  </si>
+  <si>
+    <t>CT57</t>
+  </si>
+  <si>
+    <t>CT58</t>
+  </si>
+  <si>
+    <t>CT59</t>
+  </si>
+  <si>
+    <t>CT60</t>
+  </si>
+  <si>
+    <t>CT61</t>
+  </si>
+  <si>
+    <t>CT62</t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Card Desconto para iniciante</t>
+  </si>
+  <si>
+    <t>Validar que o  status do card é "Pendente"</t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Card Desconto por direção</t>
+  </si>
+  <si>
+    <t>Validar que o status  da progress bar é "0/20" e "0/300"</t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Card Desconto de amizade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validar que o status  da progress bar é "0/3" </t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Card Agenda do carro</t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Card Check up do carro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validar que o status  da progress bar é "0/15" </t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Card Smiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validar que o status  da progress bar é "Fechar seguro com desconto de direção" </t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Brinde Iniciante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validar que o status  do brinde é "Pendente" </t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Brinde Direção</t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Brinde Amizade</t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Brinde Agenda</t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Brinde Check Up</t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Brinde Smiles</t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Cupom Desconto Seguro</t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Cupom Agenda</t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Cupom Check up</t>
+  </si>
+  <si>
+    <t>Usuário sem viagem - Cupom Smiles</t>
+  </si>
+  <si>
+    <t>Login Email Manipulado 3 viagens &lt;70</t>
+  </si>
+  <si>
+    <t>Realizar login utilizando E-mail com viagens</t>
+  </si>
+  <si>
+    <t>Realizar login utilizando E-mail sem viagens</t>
+  </si>
+  <si>
+    <t>Realizar login utilizando E-mail viagens em andamento</t>
+  </si>
+  <si>
+    <t>30/07/2021</t>
+  </si>
+  <si>
+    <t>Captura tela dos cards</t>
+  </si>
+  <si>
+    <t>Captura tela dos cupons</t>
+  </si>
+  <si>
+    <t>CT63</t>
+  </si>
+  <si>
+    <t>CT64</t>
+  </si>
+  <si>
+    <t>CT65</t>
+  </si>
+  <si>
+    <t>00:00:06</t>
+  </si>
+  <si>
+    <t>28/07/2022</t>
+  </si>
+  <si>
+    <t>00:00:07</t>
+  </si>
+  <si>
+    <t>28/07/2023</t>
+  </si>
+  <si>
+    <t>00:00:08</t>
+  </si>
+  <si>
+    <t>28/07/2024</t>
+  </si>
+  <si>
+    <t>00:00:09</t>
+  </si>
+  <si>
+    <t>28/07/2025</t>
+  </si>
+  <si>
+    <t>00:00:10</t>
+  </si>
+  <si>
+    <t>28/07/2026</t>
+  </si>
+  <si>
+    <t>00:00:11</t>
+  </si>
+  <si>
+    <t>28/07/2027</t>
+  </si>
+  <si>
+    <t>00:00:13</t>
+  </si>
+  <si>
+    <t>28/07/2029</t>
+  </si>
+  <si>
+    <t>00:00:14</t>
+  </si>
+  <si>
+    <t>28/07/2030</t>
+  </si>
+  <si>
+    <t>00:00:15</t>
+  </si>
+  <si>
+    <t>28/07/2031</t>
+  </si>
+  <si>
+    <t>00:00:16</t>
+  </si>
+  <si>
+    <t>28/07/2032</t>
+  </si>
+  <si>
+    <t>00:00:17</t>
+  </si>
+  <si>
+    <t>28/07/2033</t>
+  </si>
+  <si>
+    <t>00:00:18</t>
+  </si>
+  <si>
+    <t>28/07/2034</t>
+  </si>
+  <si>
+    <t>00:00:20</t>
+  </si>
+  <si>
+    <t>28/07/2036</t>
+  </si>
+  <si>
+    <t>00:00:21</t>
+  </si>
+  <si>
+    <t>28/07/2037</t>
+  </si>
+  <si>
+    <t>00:00:22</t>
+  </si>
+  <si>
+    <t>28/07/2038</t>
+  </si>
+  <si>
+    <t>00:00:23</t>
+  </si>
+  <si>
+    <t>28/07/2039</t>
+  </si>
+  <si>
+    <t>Usuario sem viagem - Cards</t>
+  </si>
+  <si>
+    <t>Usuario sem viagem - Brindes</t>
+  </si>
+  <si>
+    <t>Usuario sem viagem - Cupons</t>
+  </si>
+  <si>
+    <t>00:00:38</t>
+  </si>
+  <si>
+    <t>02/08/2021</t>
+  </si>
+  <si>
+    <t>Selecionar o brinde 1 (Agenda do carro).  Validar tela, textos e links deste brinde. Teste Botão Car10</t>
+  </si>
+  <si>
+    <t>00:01:49</t>
+  </si>
+  <si>
+    <t>Selecionar o brinde 2 (Check Up Automotivo). Validar tela, textos e links deste brinde. Teste Botão Car10</t>
+  </si>
+  <si>
+    <t>00:00:47</t>
+  </si>
+  <si>
+    <t>efetuar reteste para refatoração ou validação de defeito</t>
+  </si>
+  <si>
+    <t>é necessário alterar a massa de dados alterada antes da execução</t>
+  </si>
+  <si>
+    <t>03/08/2021</t>
+  </si>
+  <si>
+    <t>00:01:09</t>
+  </si>
+  <si>
+    <t>1.0.0.1662005</t>
+  </si>
+  <si>
+    <t>00:01:43</t>
+  </si>
+  <si>
+    <t>00:00:57</t>
+  </si>
+  <si>
+    <t>Não esta na tela inicial</t>
+  </si>
+  <si>
     <t>Falha ao abrir manifestação</t>
   </si>
   <si>
-    <t>00:02:08</t>
-  </si>
-  <si>
-    <t>00:01:31</t>
-  </si>
-  <si>
-    <t>Falha ao concordar com os termos</t>
-  </si>
-  <si>
-    <t>Selecionar ranking geral.  Validar que ranking está vindo ordenado pelo score dos usuários. ( todos os testes de filtro, os filtros são aplicados mas não é feita validação de ordem de score)</t>
-  </si>
-  <si>
-    <t>00:00:54</t>
-  </si>
-  <si>
-    <t>00:00:48</t>
-  </si>
-  <si>
-    <t>Inicio esperado[Ínicio - 08:57 hs.] recebido[Ínicio - 18:56 hs.]</t>
-  </si>
-  <si>
-    <t>Chegada - 18:56 hs.</t>
-  </si>
-  <si>
-    <t>00:01:48</t>
-  </si>
-  <si>
-    <t>00:01:00</t>
-  </si>
-  <si>
-    <t>00:02:01</t>
-  </si>
-  <si>
-    <t>00:01:34</t>
-  </si>
-  <si>
-    <t>https://autovc.page.link/GcZk</t>
-  </si>
-  <si>
-    <t>00:00:35</t>
-  </si>
-  <si>
-    <t>00:01:16</t>
-  </si>
-  <si>
-    <t>00:01:24</t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Ordem dos cards</t>
-  </si>
-  <si>
-    <t>Validar que ao logar com um usuário novo, os cards virão na seguinte ordem: Iniciante / Direção / Amizade / Agenda do carro / Check up do carro / Smiles</t>
-  </si>
-  <si>
-    <t>CT46</t>
-  </si>
-  <si>
-    <t>CT47</t>
-  </si>
-  <si>
-    <t>CT48</t>
-  </si>
-  <si>
-    <t>CT49</t>
-  </si>
-  <si>
-    <t>CT52</t>
-  </si>
-  <si>
-    <t>CT53</t>
-  </si>
-  <si>
-    <t>CT54</t>
-  </si>
-  <si>
-    <t>CT55</t>
-  </si>
-  <si>
-    <t>CT56</t>
-  </si>
-  <si>
-    <t>CT57</t>
-  </si>
-  <si>
-    <t>CT58</t>
-  </si>
-  <si>
-    <t>CT59</t>
-  </si>
-  <si>
-    <t>CT60</t>
-  </si>
-  <si>
-    <t>CT61</t>
-  </si>
-  <si>
-    <t>CT62</t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Card Desconto para iniciante</t>
-  </si>
-  <si>
-    <t>Validar que o  status do card é "Pendente"</t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Card Desconto por direção</t>
-  </si>
-  <si>
-    <t>Validar que o status  da progress bar é "0/20" e "0/300"</t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Card Desconto de amizade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validar que o status  da progress bar é "0/3" </t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Card Agenda do carro</t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Card Check up do carro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validar que o status  da progress bar é "0/15" </t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Card Smiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validar que o status  da progress bar é "Fechar seguro com desconto de direção" </t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Brinde Iniciante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validar que o status  do brinde é "Pendente" </t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Brinde Direção</t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Brinde Amizade</t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Brinde Agenda</t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Brinde Check Up</t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Brinde Smiles</t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Cupom Desconto Seguro</t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Cupom Agenda</t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Cupom Check up</t>
-  </si>
-  <si>
-    <t>Usuário sem viagem - Cupom Smiles</t>
-  </si>
-  <si>
-    <t>Login Email Manipulado 3 viagens &lt;70</t>
-  </si>
-  <si>
-    <t>Realizar login utilizando E-mail com viagens</t>
-  </si>
-  <si>
-    <t>Realizar login utilizando E-mail sem viagens</t>
-  </si>
-  <si>
-    <t>Realizar login utilizando E-mail viagens em andamento</t>
-  </si>
-  <si>
-    <t>30/07/2021</t>
-  </si>
-  <si>
-    <t>Captura tela dos cards</t>
-  </si>
-  <si>
-    <t>Captura tela dos cupons</t>
-  </si>
-  <si>
-    <t>CT63</t>
-  </si>
-  <si>
-    <t>CT64</t>
-  </si>
-  <si>
-    <t>CT65</t>
-  </si>
-  <si>
-    <t>00:00:06</t>
-  </si>
-  <si>
-    <t>28/07/2022</t>
-  </si>
-  <si>
-    <t>00:00:07</t>
-  </si>
-  <si>
-    <t>28/07/2023</t>
-  </si>
-  <si>
-    <t>00:00:08</t>
-  </si>
-  <si>
-    <t>28/07/2024</t>
-  </si>
-  <si>
-    <t>00:00:09</t>
-  </si>
-  <si>
-    <t>28/07/2025</t>
-  </si>
-  <si>
-    <t>00:00:10</t>
-  </si>
-  <si>
-    <t>28/07/2026</t>
-  </si>
-  <si>
-    <t>00:00:11</t>
-  </si>
-  <si>
-    <t>28/07/2027</t>
-  </si>
-  <si>
-    <t>00:00:13</t>
-  </si>
-  <si>
-    <t>28/07/2029</t>
-  </si>
-  <si>
-    <t>00:00:14</t>
-  </si>
-  <si>
-    <t>28/07/2030</t>
-  </si>
-  <si>
-    <t>00:00:15</t>
-  </si>
-  <si>
-    <t>28/07/2031</t>
-  </si>
-  <si>
-    <t>00:00:16</t>
-  </si>
-  <si>
-    <t>28/07/2032</t>
-  </si>
-  <si>
-    <t>00:00:17</t>
-  </si>
-  <si>
-    <t>28/07/2033</t>
-  </si>
-  <si>
-    <t>00:00:18</t>
-  </si>
-  <si>
-    <t>28/07/2034</t>
-  </si>
-  <si>
-    <t>00:00:20</t>
-  </si>
-  <si>
-    <t>28/07/2036</t>
-  </si>
-  <si>
-    <t>00:00:21</t>
-  </si>
-  <si>
-    <t>28/07/2037</t>
-  </si>
-  <si>
-    <t>00:00:22</t>
-  </si>
-  <si>
-    <t>28/07/2038</t>
-  </si>
-  <si>
-    <t>00:00:23</t>
-  </si>
-  <si>
-    <t>28/07/2039</t>
-  </si>
-  <si>
-    <t>Usuario sem viagem - Cards</t>
-  </si>
-  <si>
-    <t>Usuario sem viagem - Brindes</t>
-  </si>
-  <si>
-    <t>Usuario sem viagem - Cupons</t>
-  </si>
-  <si>
-    <t>00:00:38</t>
-  </si>
-  <si>
-    <t>02/08/2021</t>
-  </si>
-  <si>
-    <t>Selecionar o brinde 1 (Agenda do carro).  Validar tela, textos e links deste brinde. Teste Botão Car10</t>
-  </si>
-  <si>
-    <t>00:01:49</t>
-  </si>
-  <si>
-    <t>Selecionar o brinde 2 (Check Up Automotivo). Validar tela, textos e links deste brinde. Teste Botão Car10</t>
-  </si>
-  <si>
-    <t>00:00:47</t>
-  </si>
-  <si>
-    <t>efetuar reteste para refatoração ou validação de defeito</t>
-  </si>
-  <si>
-    <t>é necessário alterar a massa de dados alterada antes da execução</t>
-  </si>
-  <si>
-    <t>03/08/2021</t>
-  </si>
-  <si>
-    <t>00:01:09</t>
-  </si>
-  <si>
-    <t>1.0.0.1662005</t>
-  </si>
-  <si>
-    <t>00:01:43</t>
-  </si>
-  <si>
-    <t>00:00:57</t>
-  </si>
-  <si>
-    <t>00:01:11</t>
+    <t>00:02:11</t>
+  </si>
+  <si>
+    <t>04/08/2021</t>
+  </si>
+  <si>
+    <t>00:00:59</t>
+  </si>
+  <si>
+    <t>00:01:03</t>
   </si>
 </sst>
 </file>
@@ -10773,7 +10782,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10936,10 +10945,10 @@
         <v>232</v>
       </c>
       <c r="H2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="I2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="J2" t="s">
         <v>133</v>
@@ -10990,7 +10999,7 @@
         <v>131</v>
       </c>
       <c r="Z2" s="92" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="AA2" s="10">
         <v>44096</v>
@@ -11022,7 +11031,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="93" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D3" t="s">
         <v>128</v>
@@ -11037,10 +11046,10 @@
         <v>232</v>
       </c>
       <c r="H3" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="J3" t="s">
         <v>133</v>
@@ -11123,7 +11132,7 @@
         <v>292</v>
       </c>
       <c r="C4" s="93" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D4" t="s">
         <v>128</v>
@@ -11138,10 +11147,10 @@
         <v>232</v>
       </c>
       <c r="H4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="J4" t="s">
         <v>133</v>
@@ -11221,10 +11230,10 @@
         <v>257</v>
       </c>
       <c r="B5" s="104" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C5" s="93" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D5" t="s">
         <v>128</v>
@@ -11242,7 +11251,7 @@
         <v>283</v>
       </c>
       <c r="I5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="J5" t="s">
         <v>133</v>
@@ -11324,7 +11333,7 @@
       <c r="B6" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="C6" s="94" t="s">
+      <c r="C6" s="74" t="s">
         <v>187</v>
       </c>
       <c r="D6" t="s">
@@ -11340,10 +11349,10 @@
         <v>232</v>
       </c>
       <c r="H6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="J6" t="s">
         <v>133</v>
@@ -11425,7 +11434,7 @@
       <c r="B7" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="94" t="s">
+      <c r="C7" s="74" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
@@ -11444,7 +11453,7 @@
         <v>284</v>
       </c>
       <c r="I7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="J7" t="s">
         <v>133</v>
@@ -11536,16 +11545,16 @@
         <v>111</v>
       </c>
       <c r="F8" t="s">
-        <v>288</v>
+        <v>413</v>
       </c>
       <c r="G8" t="s">
         <v>231</v>
       </c>
       <c r="H8" t="s">
-        <v>240</v>
+        <v>286</v>
       </c>
       <c r="I8" t="s">
-        <v>289</v>
+        <v>408</v>
       </c>
       <c r="J8" t="s">
         <v>133</v>
@@ -12430,7 +12439,7 @@
         <v>42</v>
       </c>
       <c r="C17" s="74" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D17" t="s">
         <v>128</v>
@@ -12445,10 +12454,10 @@
         <v>232</v>
       </c>
       <c r="H17" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I17" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J17" t="s">
         <v>133</v>
@@ -12531,7 +12540,7 @@
         <v>43</v>
       </c>
       <c r="C18" s="74" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D18" t="s">
         <v>128</v>
@@ -12546,10 +12555,10 @@
         <v>232</v>
       </c>
       <c r="H18" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I18" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J18" t="s">
         <v>133</v>
@@ -12647,10 +12656,10 @@
         <v>232</v>
       </c>
       <c r="H19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="I19" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J19" t="s">
         <v>133</v>
@@ -12736,28 +12745,28 @@
         <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>111</v>
       </c>
       <c r="F20" t="s">
-        <v>304</v>
+        <v>111</v>
       </c>
       <c r="G20" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H20" t="s">
-        <v>415</v>
+        <v>314</v>
       </c>
       <c r="I20" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="J20" t="s">
         <v>133</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L20" s="22" t="s">
         <v>129</v>
@@ -12834,7 +12843,7 @@
         <v>50</v>
       </c>
       <c r="C21" s="97" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D21" t="s">
         <v>128</v>
@@ -12849,7 +12858,7 @@
         <v>232</v>
       </c>
       <c r="H21" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I21" t="s">
         <v>294</v>
@@ -13247,7 +13256,7 @@
         <v>111</v>
       </c>
       <c r="F25" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G25" t="s">
         <v>231</v>
@@ -13455,7 +13464,7 @@
         <v>232</v>
       </c>
       <c r="H27" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I27" t="s">
         <v>294</v>
@@ -13556,7 +13565,7 @@
         <v>232</v>
       </c>
       <c r="H28" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I28" t="s">
         <v>294</v>
@@ -13648,16 +13657,16 @@
         <v>128</v>
       </c>
       <c r="E29" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F29" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G29" t="s">
         <v>232</v>
       </c>
       <c r="H29" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I29" t="s">
         <v>294</v>
@@ -13723,7 +13732,7 @@
         <v>276</v>
       </c>
       <c r="AD29" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AE29" s="7" t="s">
         <v>277</v>
@@ -13758,7 +13767,7 @@
         <v>232</v>
       </c>
       <c r="H30" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I30" t="s">
         <v>294</v>
@@ -14098,7 +14107,7 @@
         <v>232</v>
       </c>
       <c r="H34" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I34" t="s">
         <v>294</v>
@@ -14298,7 +14307,7 @@
         <v>232</v>
       </c>
       <c r="H36" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I36" t="s">
         <v>294</v>
@@ -14399,7 +14408,7 @@
         <v>232</v>
       </c>
       <c r="H37" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I37" t="s">
         <v>294</v>
@@ -14420,7 +14429,7 @@
         <v>131</v>
       </c>
       <c r="O37" s="79" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="P37" s="7" t="s">
         <v>131</v>
@@ -14601,7 +14610,7 @@
         <v>231</v>
       </c>
       <c r="H39" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I39" t="s">
         <v>294</v>
@@ -14904,7 +14913,7 @@
         <v>232</v>
       </c>
       <c r="H42" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I42" t="s">
         <v>294</v>
@@ -15102,7 +15111,7 @@
         <v>232</v>
       </c>
       <c r="H44" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I44" t="s">
         <v>294</v>
@@ -15180,13 +15189,13 @@
     </row>
     <row r="47" spans="1:33">
       <c r="A47" s="107" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B47" s="105" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C47" s="105" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D47" t="s">
         <v>128</v>
@@ -15204,7 +15213,7 @@
         <v>240</v>
       </c>
       <c r="I47" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J47" t="s">
         <v>133</v>
@@ -15281,13 +15290,13 @@
     </row>
     <row r="48" spans="1:33">
       <c r="A48" s="14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B48" s="105" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C48" s="105" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D48" t="s">
         <v>128</v>
@@ -15382,13 +15391,13 @@
     </row>
     <row r="49" spans="1:33">
       <c r="A49" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B49" s="105" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C49" s="105" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D49" t="s">
         <v>128</v>
@@ -15403,10 +15412,10 @@
         <v>231</v>
       </c>
       <c r="H49" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I49" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J49" t="s">
         <v>133</v>
@@ -15483,13 +15492,13 @@
     </row>
     <row r="50" spans="1:33">
       <c r="A50" s="14" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B50" s="105" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C50" s="105" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D50" t="s">
         <v>128</v>
@@ -15504,10 +15513,10 @@
         <v>231</v>
       </c>
       <c r="H50" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I50" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="J50" t="s">
         <v>133</v>
@@ -15587,10 +15596,10 @@
         <v>60</v>
       </c>
       <c r="B51" s="105" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C51" s="105" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D51" t="s">
         <v>128</v>
@@ -15605,10 +15614,10 @@
         <v>231</v>
       </c>
       <c r="H51" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I51" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J51" t="s">
         <v>133</v>
@@ -15688,10 +15697,10 @@
         <v>61</v>
       </c>
       <c r="B52" s="105" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C52" s="105" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D52" t="s">
         <v>128</v>
@@ -15706,10 +15715,10 @@
         <v>231</v>
       </c>
       <c r="H52" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I52" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J52" t="s">
         <v>133</v>
@@ -15786,13 +15795,13 @@
     </row>
     <row r="53" spans="1:33">
       <c r="A53" s="14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B53" s="105" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C53" s="105" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D53" t="s">
         <v>128</v>
@@ -15807,10 +15816,10 @@
         <v>231</v>
       </c>
       <c r="H53" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="I53" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J53" t="s">
         <v>133</v>
@@ -15887,13 +15896,13 @@
     </row>
     <row r="54" spans="1:33">
       <c r="A54" s="14" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B54" s="105" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C54" s="105" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D54" t="s">
         <v>128</v>
@@ -15908,10 +15917,10 @@
         <v>231</v>
       </c>
       <c r="H54" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="I54" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J54" t="s">
         <v>133</v>
@@ -15988,13 +15997,13 @@
     </row>
     <row r="55" spans="1:33">
       <c r="A55" s="107" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B55" s="106" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C55" s="106" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D55" t="s">
         <v>128</v>
@@ -16012,7 +16021,7 @@
         <v>269</v>
       </c>
       <c r="I55" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J55" t="s">
         <v>133</v>
@@ -16089,13 +16098,13 @@
     </row>
     <row r="56" spans="1:33">
       <c r="A56" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B56" s="106" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C56" s="106" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D56" t="s">
         <v>128</v>
@@ -16110,10 +16119,10 @@
         <v>231</v>
       </c>
       <c r="H56" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I56" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J56" t="s">
         <v>133</v>
@@ -16190,13 +16199,13 @@
     </row>
     <row r="57" spans="1:33">
       <c r="A57" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B57" s="106" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C57" s="106" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D57" t="s">
         <v>128</v>
@@ -16211,10 +16220,10 @@
         <v>231</v>
       </c>
       <c r="H57" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="I57" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="J57" t="s">
         <v>133</v>
@@ -16291,13 +16300,13 @@
     </row>
     <row r="58" spans="1:33">
       <c r="A58" s="108" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B58" s="106" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C58" s="106" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D58" t="s">
         <v>128</v>
@@ -16312,10 +16321,10 @@
         <v>231</v>
       </c>
       <c r="H58" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I58" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="J58" t="s">
         <v>133</v>
@@ -16392,13 +16401,13 @@
     </row>
     <row r="59" spans="1:33">
       <c r="A59" s="14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B59" s="106" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C59" s="106" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D59" t="s">
         <v>128</v>
@@ -16413,10 +16422,10 @@
         <v>231</v>
       </c>
       <c r="H59" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I59" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J59" t="s">
         <v>133</v>
@@ -16493,13 +16502,13 @@
     </row>
     <row r="60" spans="1:33">
       <c r="A60" s="14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B60" s="106" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C60" s="106" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D60" t="s">
         <v>128</v>
@@ -16514,10 +16523,10 @@
         <v>231</v>
       </c>
       <c r="H60" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I60" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="J60" t="s">
         <v>133</v>
@@ -16594,13 +16603,13 @@
     </row>
     <row r="61" spans="1:33">
       <c r="A61" s="14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B61" s="106" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C61" s="106" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D61" t="s">
         <v>128</v>
@@ -16615,10 +16624,10 @@
         <v>231</v>
       </c>
       <c r="H61" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I61" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="J61" t="s">
         <v>133</v>
@@ -16695,13 +16704,13 @@
     </row>
     <row r="62" spans="1:33">
       <c r="A62" s="107" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B62" s="105" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C62" s="105" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D62" t="s">
         <v>128</v>
@@ -16716,10 +16725,10 @@
         <v>232</v>
       </c>
       <c r="H62" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I62" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J62" t="s">
         <v>133</v>
@@ -16796,13 +16805,13 @@
     </row>
     <row r="63" spans="1:33">
       <c r="A63" s="14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B63" s="105" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C63" s="105" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D63" t="s">
         <v>128</v>
@@ -16817,10 +16826,10 @@
         <v>231</v>
       </c>
       <c r="H63" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I63" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="J63" t="s">
         <v>133</v>
@@ -16897,13 +16906,13 @@
     </row>
     <row r="64" spans="1:33">
       <c r="A64" s="14" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B64" s="105" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C64" s="105" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D64" t="s">
         <v>128</v>
@@ -16918,10 +16927,10 @@
         <v>231</v>
       </c>
       <c r="H64" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I64" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J64" t="s">
         <v>133</v>
@@ -16998,13 +17007,13 @@
     </row>
     <row r="65" spans="1:35">
       <c r="A65" s="14" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B65" s="105" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C65" s="105" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D65" t="s">
         <v>128</v>
@@ -17019,10 +17028,10 @@
         <v>231</v>
       </c>
       <c r="H65" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I65" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J65" t="s">
         <v>133</v>
@@ -17099,13 +17108,13 @@
     </row>
     <row r="66" spans="1:35">
       <c r="A66" s="14" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B66" s="105" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C66" s="105" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D66" t="s">
         <v>128</v>
@@ -17120,10 +17129,10 @@
         <v>231</v>
       </c>
       <c r="H66" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I66" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="J66" t="s">
         <v>133</v>
@@ -17235,13 +17244,13 @@
     <row r="68" spans="1:35">
       <c r="B68" s="111"/>
       <c r="C68" s="110" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="69" spans="1:35">
       <c r="B69" s="98"/>
       <c r="C69" s="98" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="AI69" s="40"/>
     </row>

</xml_diff>

<commit_message>
missões não cumpridas 20 viagens score <70
</commit_message>
<xml_diff>
--- a/data/AutoVC.xlsx
+++ b/data/AutoVC.xlsx
@@ -15,8 +15,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Testes!$A$1:$AG$54</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT([0]!LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3" hidden="1"><![CDATA[REPT(LOCAL_YEAR_FORMAT,4)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_MONTH_FORMAT,2)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_DAY_FORMAT,2)&" "&REPT(LOCAL_HOUR_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT(LOCAL_MINUTE_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT([0]!LOCAL_SECOND_FORMAT,2)]]></definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1"><![CDATA[REPT(LOCAL_YEAR_FORMAT,4)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_MONTH_FORMAT,2)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_DAY_FORMAT,2)&" "&REPT(LOCAL_HOUR_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT(LOCAL_MINUTE_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT(LOCAL_SECOND_FORMAT,2)]]></definedName>
     <definedName name="LOCAL_SECOND_FORMAT" hidden="1">" "</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2342" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2380" uniqueCount="430">
   <si>
     <t>Telefone</t>
   </si>
@@ -1396,6 +1396,21 @@
   </si>
   <si>
     <t>samtesteaz03@gmail.com</t>
+  </si>
+  <si>
+    <t>00:01:15</t>
+  </si>
+  <si>
+    <t>Cards desconto por direção, amizade e 800 milhas não cumprida</t>
+  </si>
+  <si>
+    <t>Usuario 20 viagens score &lt;70 - Missoes Não Cumpridas</t>
+  </si>
+  <si>
+    <t>00:00:39</t>
+  </si>
+  <si>
+    <t>00:00:41</t>
   </si>
 </sst>
 </file>
@@ -2109,6 +2124,46 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -2139,63 +2194,23 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -9832,46 +9847,46 @@
   <sheetPr codeName="Plan3"/>
   <dimension ref="A1:AI88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.7109375" style="9" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="121.140625" style="73" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.5703125" style="29" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="43.5703125" style="9" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="35.7109375" style="9" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.7109375" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.7109375" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="12.7109375" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="26.85546875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.140625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23.28515625" style="9" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="8.28515625" style="9" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="23.5703125" style="9" customWidth="1" collapsed="1"/>
-    <col min="19" max="20" width="15" style="9" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="15.140625" style="9" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="23.85546875" style="9" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="24.5703125" style="9" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="19.140625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="17.5703125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="25.7109375" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="17.7109375" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="19.28515625" style="9" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="14" style="13" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.28515625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="16384" width="9.140625" style="13" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="7.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="9" width="49.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="73" width="121.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="29" width="9.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="9" width="43.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="9" width="35.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="9" width="11.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="9" width="11.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="9" width="14.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="7" width="10.7109375" collapsed="true"/>
+    <col min="11" max="12" bestFit="true" customWidth="true" style="9" width="12.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="9" width="26.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="9" width="15.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="9" width="23.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="9" width="8.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="9" width="12.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="9" width="23.5703125" collapsed="true"/>
+    <col min="19" max="20" customWidth="true" style="9" width="15.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="9" width="12.0" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="9" width="15.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="9" width="13.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="9" width="23.85546875" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="9" width="24.5703125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="9" width="19.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="9" width="17.5703125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="9" width="25.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="9" width="17.7109375" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="9" width="19.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="9" width="24.0" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="13" width="14.0" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="13" width="15.28515625" collapsed="true"/>
+    <col min="34" max="16384" style="13" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" s="12" customFormat="1">
@@ -10895,7 +10910,7 @@
         <v>423</v>
       </c>
       <c r="D11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>110</v>
@@ -10907,10 +10922,10 @@
         <v>231</v>
       </c>
       <c r="H11" t="s">
-        <v>401</v>
+        <v>425</v>
       </c>
       <c r="I11" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="J11" t="s">
         <v>132</v>
@@ -10986,38 +11001,105 @@
       </c>
     </row>
     <row r="12" spans="1:33">
-      <c r="A12" s="14"/>
-      <c r="B12" s="104"/>
-      <c r="C12" s="93"/>
-      <c r="D12"/>
-      <c r="E12" s="5"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="90"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="7"/>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="7"/>
-      <c r="AC12" s="7"/>
-      <c r="AD12" s="7"/>
-      <c r="AE12" s="7"/>
-      <c r="AF12" s="7"/>
-      <c r="AG12" s="7"/>
+      <c r="A12" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>427</v>
+      </c>
+      <c r="C12" s="93" t="s">
+        <v>426</v>
+      </c>
+      <c r="D12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H12" t="s">
+        <v>429</v>
+      </c>
+      <c r="I12" t="s">
+        <v>406</v>
+      </c>
+      <c r="J12" t="s">
+        <v>132</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="M12" s="90" t="s">
+        <v>424</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="R12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="T12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="U12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="V12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="W12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="X12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG12" s="7" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="13" spans="1:33">
       <c r="A13" s="14" t="s">
@@ -16605,3214 +16687,3243 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AG54"/>
-  <conditionalFormatting sqref="I16 F18:H18 F13:H14 F49:H49 G48:I48 F32:H33 G16:H22 F42:I47 F36:I40 F54:I60 F62:I67 F69:I73 F5:I6 F20:H30 F10:I10 F12:I12">
-    <cfRule type="containsText" dxfId="802" priority="2445" operator="containsText" text="Passed">
+  <conditionalFormatting sqref="I16 F18:H18 F13:H14 F49:H49 G48:I48 F32:H33 G16:H22 F42:I47 F36:I40 F54:I60 F62:I67 F69:I73 F5:I6 F20:H30 F10:I10">
+    <cfRule type="containsText" dxfId="802" priority="2452" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="801" priority="2446" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="801" priority="2453" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40">
-    <cfRule type="containsText" dxfId="800" priority="2437" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="800" priority="2444" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="799" priority="2438" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="799" priority="2445" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="containsText" dxfId="798" priority="2429" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="798" priority="2436" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="797" priority="2430" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="797" priority="2437" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="containsText" dxfId="796" priority="2421" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="796" priority="2428" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="795" priority="2422" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="795" priority="2429" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="containsText" dxfId="794" priority="2417" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="794" priority="2424" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="793" priority="2418" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="793" priority="2425" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="containsText" dxfId="792" priority="2409" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="792" priority="2416" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="791" priority="2410" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="791" priority="2417" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:I20">
-    <cfRule type="containsText" dxfId="790" priority="2401" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="790" priority="2408" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="789" priority="2402" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="789" priority="2409" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="788" priority="2397" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="788" priority="2404" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="787" priority="2398" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="787" priority="2405" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="containsText" dxfId="786" priority="2393" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="786" priority="2400" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="785" priority="2394" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="785" priority="2401" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42">
-    <cfRule type="containsText" dxfId="784" priority="2389" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="784" priority="2396" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="783" priority="2390" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="783" priority="2397" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="containsText" dxfId="782" priority="2385" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="782" priority="2392" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="781" priority="2386" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="781" priority="2393" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="containsText" dxfId="780" priority="2381" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="780" priority="2388" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="779" priority="2382" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="779" priority="2389" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26">
-    <cfRule type="containsText" dxfId="778" priority="2377" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="778" priority="2384" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="777" priority="2378" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="777" priority="2385" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="containsText" dxfId="776" priority="2371" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="776" priority="2378" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="775" priority="2372" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="775" priority="2379" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28">
-    <cfRule type="containsText" dxfId="774" priority="2367" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="774" priority="2374" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="773" priority="2368" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="773" priority="2375" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29">
-    <cfRule type="containsText" dxfId="772" priority="2363" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="772" priority="2370" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="771" priority="2364" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="771" priority="2371" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43">
-    <cfRule type="containsText" dxfId="770" priority="2359" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="770" priority="2366" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="769" priority="2360" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="769" priority="2367" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I44">
-    <cfRule type="containsText" dxfId="768" priority="2351" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="768" priority="2358" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I44)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="767" priority="2352" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="767" priority="2359" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47">
-    <cfRule type="containsText" dxfId="766" priority="2343" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="766" priority="2350" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="765" priority="2344" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="765" priority="2351" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45">
-    <cfRule type="containsText" dxfId="764" priority="2339" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="764" priority="2346" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="763" priority="2340" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="763" priority="2347" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25">
-    <cfRule type="containsText" dxfId="762" priority="2331" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="762" priority="2338" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="761" priority="2332" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="761" priority="2339" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="containsText" dxfId="760" priority="2327" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="760" priority="2334" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="759" priority="2328" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="759" priority="2335" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="containsText" dxfId="758" priority="2323" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="758" priority="2330" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="757" priority="2324" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="757" priority="2331" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="containsText" dxfId="756" priority="2319" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="756" priority="2326" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="755" priority="2320" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="755" priority="2327" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:I37">
-    <cfRule type="containsText" dxfId="754" priority="2315" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="754" priority="2322" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="753" priority="2316" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="753" priority="2323" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38:I39">
-    <cfRule type="containsText" dxfId="752" priority="2311" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="752" priority="2318" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="751" priority="2312" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="751" priority="2319" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46">
-    <cfRule type="containsText" dxfId="750" priority="2307" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="750" priority="2314" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="749" priority="2308" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="749" priority="2315" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="containsText" dxfId="748" priority="2271" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="748" priority="2278" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="747" priority="2272" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="747" priority="2279" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K44:L45 K49:L49 L32:L33 L42 L36:L40 D26:D50 L25:L30 K25 K54:L60 D54:D60 K62:L67 K69:L73 K5:L6 D62:D67 D69:D73 D5:D6 K16:L24 K10:L10 D10 D12:D22 K12:L14">
-    <cfRule type="containsText" dxfId="746" priority="2263" operator="containsText" text="Sim">
+  <conditionalFormatting sqref="K44:L45 K49:L49 L32:L33 L42 L36:L40 D26:D50 L25:L30 K25 K54:L60 D54:D60 K62:L67 K69:L73 K5:L6 D62:D67 D69:D73 D5:D6 K16:L24 K10:L10 D10 D13:D22 K13:L14">
+    <cfRule type="containsText" dxfId="746" priority="2270" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="745" priority="2264" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="745" priority="2271" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:K33">
-    <cfRule type="containsText" dxfId="744" priority="2159" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="744" priority="2166" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="743" priority="2160" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="743" priority="2167" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K32)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J16:J17 J32:J33 J42 J36:J40 J54:J60 J62:J67 J69:J73 J5:J6 J19:J30 J10 J12:J14">
-    <cfRule type="containsText" dxfId="742" priority="2150" operator="containsText" text="Android">
+  <conditionalFormatting sqref="J16:J17 J32:J33 J42 J36:J40 J54:J60 J62:J67 J69:J73 J5:J6 J19:J30 J10 J13:J14">
+    <cfRule type="containsText" dxfId="742" priority="2157" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J16:J17 J32:J33 J42 J36:J40 J54:J60 J62:J67 J69:J73 J5:J6 J19:J30 J10 J12:J14">
-    <cfRule type="containsText" dxfId="741" priority="2148" operator="containsText" text="Web">
+  <conditionalFormatting sqref="J16:J17 J32:J33 J42 J36:J40 J54:J60 J62:J67 J69:J73 J5:J6 J19:J30 J10 J13:J14">
+    <cfRule type="containsText" dxfId="741" priority="2155" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="740" priority="2149" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="740" priority="2156" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44">
-    <cfRule type="containsText" dxfId="739" priority="2141" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="739" priority="2148" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44">
-    <cfRule type="containsText" dxfId="738" priority="2139" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="738" priority="2146" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J44)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="737" priority="2140" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="737" priority="2147" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45">
-    <cfRule type="containsText" dxfId="736" priority="2138" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="736" priority="2145" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45">
-    <cfRule type="containsText" dxfId="735" priority="2136" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="735" priority="2143" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="734" priority="2137" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="734" priority="2144" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49">
-    <cfRule type="containsText" dxfId="733" priority="2123" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="733" priority="2130" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49">
-    <cfRule type="containsText" dxfId="732" priority="2121" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="732" priority="2128" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="731" priority="2122" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="731" priority="2129" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43">
-    <cfRule type="containsText" dxfId="730" priority="2120" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="730" priority="2127" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43">
-    <cfRule type="containsText" dxfId="729" priority="2118" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="729" priority="2125" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="728" priority="2119" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="728" priority="2126" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J47">
-    <cfRule type="containsText" dxfId="727" priority="2114" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="727" priority="2121" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J47">
-    <cfRule type="containsText" dxfId="726" priority="2112" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="726" priority="2119" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="725" priority="2113" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="725" priority="2120" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="containsText" dxfId="724" priority="2106" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="724" priority="2113" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="723" priority="2107" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="723" priority="2114" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="722" priority="2104" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="722" priority="2111" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="721" priority="2105" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="721" priority="2112" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38:K39">
-    <cfRule type="containsText" dxfId="720" priority="2102" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="720" priority="2109" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="719" priority="2103" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="719" priority="2110" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:K37">
-    <cfRule type="containsText" dxfId="718" priority="2100" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="718" priority="2107" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="717" priority="2101" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="717" priority="2108" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J46">
-    <cfRule type="containsText" dxfId="716" priority="2099" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="716" priority="2106" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J46">
-    <cfRule type="containsText" dxfId="715" priority="2097" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="715" priority="2104" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="714" priority="2098" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="714" priority="2105" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="containsText" dxfId="713" priority="2093" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="713" priority="2100" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",L46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="712" priority="2094" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="712" priority="2101" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",L46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46">
-    <cfRule type="containsText" dxfId="711" priority="2003" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="711" priority="2010" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="710" priority="2004" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="710" priority="2011" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="containsText" dxfId="709" priority="1999" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="709" priority="2006" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",H48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="708" priority="2000" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="708" priority="2007" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",H48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48">
-    <cfRule type="containsText" dxfId="707" priority="1997" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="707" priority="2004" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="706" priority="1998" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="706" priority="2005" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L48">
-    <cfRule type="containsText" dxfId="705" priority="1995" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="705" priority="2002" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",L48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="704" priority="1996" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="704" priority="2003" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",L48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48">
-    <cfRule type="containsText" dxfId="703" priority="1993" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="703" priority="2000" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="702" priority="1994" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="702" priority="2001" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48">
-    <cfRule type="containsText" dxfId="701" priority="1992" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="701" priority="1999" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48">
-    <cfRule type="containsText" dxfId="700" priority="1990" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="700" priority="1997" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="699" priority="1991" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="699" priority="1998" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48">
-    <cfRule type="containsText" dxfId="698" priority="1969" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="698" priority="1976" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",G48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="697" priority="1970" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="697" priority="1977" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",G48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:H15">
-    <cfRule type="containsText" dxfId="696" priority="1956" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="696" priority="1963" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",G15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="695" priority="1957" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="695" priority="1964" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",G15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15 I15">
-    <cfRule type="containsText" dxfId="694" priority="1952" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="694" priority="1959" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="693" priority="1953" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="693" priority="1960" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:L15">
-    <cfRule type="containsText" dxfId="692" priority="1950" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="692" priority="1957" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="691" priority="1951" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="691" priority="1958" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="containsText" dxfId="690" priority="1949" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="690" priority="1956" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="containsText" dxfId="689" priority="1947" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="689" priority="1954" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="688" priority="1948" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="688" priority="1955" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:H34">
-    <cfRule type="containsText" dxfId="687" priority="1924" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="687" priority="1931" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="686" priority="1925" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="686" priority="1932" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34">
-    <cfRule type="containsText" dxfId="685" priority="1922" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="685" priority="1929" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="684" priority="1923" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="684" priority="1930" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L34">
-    <cfRule type="containsText" dxfId="683" priority="1920" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="683" priority="1927" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",L34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="682" priority="1921" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="682" priority="1928" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",L34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="containsText" dxfId="681" priority="1918" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="681" priority="1925" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="680" priority="1919" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="680" priority="1926" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J34">
-    <cfRule type="containsText" dxfId="679" priority="1917" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="679" priority="1924" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J34">
-    <cfRule type="containsText" dxfId="678" priority="1915" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="678" priority="1922" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="677" priority="1916" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="677" priority="1923" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31:H31">
-    <cfRule type="containsText" dxfId="676" priority="1913" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="676" priority="1920" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="675" priority="1914" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="675" priority="1921" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31">
-    <cfRule type="containsText" dxfId="674" priority="1911" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="674" priority="1918" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="673" priority="1912" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="673" priority="1919" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L31">
-    <cfRule type="containsText" dxfId="672" priority="1909" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="672" priority="1916" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",L31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="671" priority="1910" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="671" priority="1917" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",L31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="containsText" dxfId="670" priority="1907" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="670" priority="1914" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="669" priority="1908" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="669" priority="1915" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
-    <cfRule type="containsText" dxfId="668" priority="1906" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="668" priority="1913" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
-    <cfRule type="containsText" dxfId="667" priority="1904" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="667" priority="1911" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="666" priority="1905" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="666" priority="1912" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="containsText" dxfId="665" priority="1896" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="665" priority="1903" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="664" priority="1897" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="664" priority="1904" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27">
-    <cfRule type="containsText" dxfId="663" priority="1894" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="663" priority="1901" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="662" priority="1895" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="662" priority="1902" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F50:H50">
-    <cfRule type="containsText" dxfId="661" priority="1892" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="661" priority="1899" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="660" priority="1893" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="660" priority="1900" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50">
-    <cfRule type="containsText" dxfId="659" priority="1890" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="659" priority="1897" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="658" priority="1891" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="658" priority="1898" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="containsText" dxfId="657" priority="1886" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="657" priority="1893" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",L50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="656" priority="1887" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="656" priority="1894" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",L50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K50">
-    <cfRule type="containsText" dxfId="655" priority="1884" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="655" priority="1891" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="654" priority="1885" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="654" priority="1892" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J50">
-    <cfRule type="containsText" dxfId="653" priority="1883" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="653" priority="1890" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J50">
-    <cfRule type="containsText" dxfId="652" priority="1881" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="652" priority="1888" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="651" priority="1882" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="651" priority="1889" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47">
-    <cfRule type="containsText" dxfId="650" priority="1846" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="650" priority="1853" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",G47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="649" priority="1847" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="649" priority="1854" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",G47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="containsText" dxfId="648" priority="1840" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="648" priority="1847" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",E50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="647" priority="1841" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="647" priority="1848" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",E50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40">
-    <cfRule type="containsText" dxfId="646" priority="1838" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="646" priority="1845" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="645" priority="1839" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="645" priority="1846" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="644" priority="1778" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="644" priority="1785" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="643" priority="1779" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="643" priority="1786" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="containsText" dxfId="642" priority="1776" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="642" priority="1783" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="641" priority="1777" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="641" priority="1784" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="containsText" dxfId="640" priority="1774" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="640" priority="1781" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="639" priority="1775" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="639" priority="1782" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:H35">
-    <cfRule type="containsText" dxfId="638" priority="1772" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="638" priority="1779" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="637" priority="1773" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="637" priority="1780" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="containsText" dxfId="636" priority="1770" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="636" priority="1777" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="635" priority="1771" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="635" priority="1778" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35">
-    <cfRule type="containsText" dxfId="634" priority="1768" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="634" priority="1775" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",L35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="633" priority="1769" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="633" priority="1776" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",L35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35">
-    <cfRule type="containsText" dxfId="632" priority="1766" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="632" priority="1773" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="631" priority="1767" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="631" priority="1774" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35">
-    <cfRule type="containsText" dxfId="630" priority="1765" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="630" priority="1772" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35">
-    <cfRule type="containsText" dxfId="629" priority="1763" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="629" priority="1770" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="628" priority="1764" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="628" priority="1771" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41:I41">
-    <cfRule type="containsText" dxfId="627" priority="1747" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="627" priority="1754" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="626" priority="1748" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="626" priority="1755" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41">
-    <cfRule type="containsText" dxfId="625" priority="1745" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="625" priority="1752" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="624" priority="1746" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="624" priority="1753" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L41">
-    <cfRule type="containsText" dxfId="623" priority="1743" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="623" priority="1750" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",L41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="622" priority="1744" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="622" priority="1751" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",L41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="containsText" dxfId="621" priority="1742" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="621" priority="1749" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="containsText" dxfId="620" priority="1740" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="620" priority="1747" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="619" priority="1741" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="619" priority="1748" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="containsText" dxfId="618" priority="1732" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="618" priority="1739" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="617" priority="1733" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="617" priority="1740" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K41">
-    <cfRule type="containsText" dxfId="616" priority="1697" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="616" priority="1704" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="615" priority="1698" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="615" priority="1705" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="containsText" dxfId="614" priority="960" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="614" priority="967" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="613" priority="961" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="613" priority="968" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="containsText" dxfId="612" priority="958" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="612" priority="965" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="611" priority="959" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="611" priority="966" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="containsText" dxfId="610" priority="956" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="610" priority="963" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",L2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="609" priority="957" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="609" priority="964" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2">
-    <cfRule type="containsText" dxfId="608" priority="955" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="608" priority="962" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2">
-    <cfRule type="containsText" dxfId="607" priority="953" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="607" priority="960" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="606" priority="954" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="606" priority="961" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="containsText" dxfId="605" priority="951" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="605" priority="958" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="604" priority="952" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="604" priority="959" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="containsText" dxfId="603" priority="949" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="603" priority="956" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="602" priority="950" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="602" priority="957" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="601" priority="947" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="601" priority="954" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="600" priority="948" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="600" priority="955" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="599" priority="945" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="599" priority="952" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="598" priority="946" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="598" priority="953" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="597" priority="943" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="597" priority="950" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="596" priority="944" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="596" priority="951" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="595" priority="941" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="595" priority="948" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="594" priority="942" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="594" priority="949" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="593" priority="939" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="593" priority="946" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="592" priority="940" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="592" priority="947" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="591" priority="937" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="591" priority="944" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="590" priority="938" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="590" priority="945" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="589" priority="935" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="589" priority="942" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="588" priority="936" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="588" priority="943" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="587" priority="933" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="587" priority="940" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="586" priority="934" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="586" priority="941" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="585" priority="931" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="585" priority="938" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="584" priority="932" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="584" priority="939" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="583" priority="929" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="583" priority="936" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="582" priority="930" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="582" priority="937" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="581" priority="927" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="581" priority="934" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="580" priority="928" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="580" priority="935" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="579" priority="925" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="579" priority="932" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="578" priority="926" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="578" priority="933" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="577" priority="923" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="577" priority="930" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="576" priority="924" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="576" priority="931" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="575" priority="921" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="575" priority="928" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="574" priority="922" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="574" priority="929" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="573" priority="919" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="573" priority="926" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="572" priority="920" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="572" priority="927" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="571" priority="917" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="571" priority="924" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="570" priority="918" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="570" priority="925" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="569" priority="915" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="569" priority="922" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="568" priority="916" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="568" priority="923" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="567" priority="913" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="567" priority="920" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="566" priority="914" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="566" priority="921" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="565" priority="911" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="565" priority="918" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="564" priority="912" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="564" priority="919" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="563" priority="909" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="563" priority="916" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="562" priority="910" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="562" priority="917" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="561" priority="907" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="561" priority="914" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="560" priority="908" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="560" priority="915" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="559" priority="905" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="559" priority="912" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="558" priority="906" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="558" priority="913" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="557" priority="903" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="557" priority="910" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="556" priority="904" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="556" priority="911" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="555" priority="901" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="555" priority="908" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="554" priority="902" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="554" priority="909" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="553" priority="899" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="553" priority="906" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="552" priority="900" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="552" priority="907" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="551" priority="897" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="551" priority="904" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="550" priority="898" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="550" priority="905" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="549" priority="895" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="549" priority="902" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="548" priority="896" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="548" priority="903" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="547" priority="776" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="547" priority="783" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="546" priority="777" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="546" priority="784" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="545" priority="774" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="545" priority="781" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="544" priority="775" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="544" priority="782" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="543" priority="772" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="543" priority="779" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="542" priority="773" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="542" priority="780" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="541" priority="770" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="541" priority="777" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="540" priority="771" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="540" priority="778" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="539" priority="768" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="539" priority="775" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="538" priority="769" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="538" priority="776" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="537" priority="766" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="537" priority="773" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="536" priority="767" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="536" priority="774" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="535" priority="764" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="535" priority="771" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="534" priority="765" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="534" priority="772" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="533" priority="762" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="533" priority="769" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="532" priority="763" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="532" priority="770" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="531" priority="760" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="531" priority="767" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="530" priority="761" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="530" priority="768" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="529" priority="758" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="529" priority="765" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="528" priority="759" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="528" priority="766" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="527" priority="756" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="527" priority="763" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="526" priority="757" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="526" priority="764" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="525" priority="754" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="525" priority="761" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="524" priority="755" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="524" priority="762" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="523" priority="752" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="523" priority="759" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="522" priority="753" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="522" priority="760" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="521" priority="750" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="521" priority="757" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="520" priority="751" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="520" priority="758" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="519" priority="748" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="519" priority="755" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="518" priority="749" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="518" priority="756" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="517" priority="746" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="517" priority="753" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="516" priority="747" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="516" priority="754" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="515" priority="744" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="515" priority="751" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="514" priority="745" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="514" priority="752" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="513" priority="742" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="513" priority="749" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="512" priority="743" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="512" priority="750" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="511" priority="740" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="511" priority="747" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="510" priority="741" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="510" priority="748" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="509" priority="738" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="509" priority="745" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="508" priority="739" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="508" priority="746" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="507" priority="736" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="507" priority="743" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="506" priority="737" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="506" priority="744" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="505" priority="734" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="505" priority="741" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="504" priority="735" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="504" priority="742" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="503" priority="732" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="503" priority="739" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="502" priority="733" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="502" priority="740" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="501" priority="730" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="501" priority="737" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="500" priority="731" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="500" priority="738" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="499" priority="728" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="499" priority="735" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="498" priority="729" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="498" priority="736" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="497" priority="726" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="497" priority="733" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="496" priority="727" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="496" priority="734" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D25">
-    <cfRule type="containsText" dxfId="495" priority="724" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="495" priority="731" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="494" priority="725" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="494" priority="732" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18">
-    <cfRule type="containsText" dxfId="493" priority="723" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="493" priority="730" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18">
-    <cfRule type="containsText" dxfId="492" priority="721" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="492" priority="728" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="491" priority="722" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="491" priority="729" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:H3">
-    <cfRule type="containsText" dxfId="490" priority="600" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="490" priority="607" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="489" priority="601" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="489" priority="608" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="containsText" dxfId="488" priority="598" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="488" priority="605" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="487" priority="599" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="487" priority="606" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L3">
-    <cfRule type="containsText" dxfId="486" priority="596" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="486" priority="603" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="485" priority="597" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="485" priority="604" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="containsText" dxfId="484" priority="595" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="484" priority="602" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="containsText" dxfId="483" priority="593" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="483" priority="600" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="482" priority="594" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="482" priority="601" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="481" priority="591" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="481" priority="598" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="480" priority="592" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="480" priority="599" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="479" priority="589" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="479" priority="596" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="478" priority="590" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="478" priority="597" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="477" priority="587" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="477" priority="594" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="476" priority="588" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="476" priority="595" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="475" priority="585" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="475" priority="592" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="474" priority="586" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="474" priority="593" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="473" priority="583" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="473" priority="590" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="472" priority="584" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="472" priority="591" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="471" priority="581" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="471" priority="588" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="470" priority="582" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="470" priority="589" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="469" priority="579" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="469" priority="586" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="468" priority="580" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="468" priority="587" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="467" priority="577" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="467" priority="584" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="466" priority="578" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="466" priority="585" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="465" priority="575" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="465" priority="582" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="464" priority="576" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="464" priority="583" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="463" priority="573" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="463" priority="580" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="462" priority="574" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="462" priority="581" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="461" priority="571" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="461" priority="578" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="460" priority="572" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="460" priority="579" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="459" priority="569" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="459" priority="576" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="458" priority="570" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="458" priority="577" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="457" priority="567" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="457" priority="574" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="456" priority="568" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="456" priority="575" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="455" priority="565" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="455" priority="572" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="454" priority="566" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="454" priority="573" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="453" priority="563" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="453" priority="570" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="452" priority="564" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="452" priority="571" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="451" priority="561" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="451" priority="568" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="450" priority="562" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="450" priority="569" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="449" priority="559" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="449" priority="566" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="448" priority="560" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="448" priority="567" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="447" priority="557" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="447" priority="564" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="446" priority="558" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="446" priority="565" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="445" priority="555" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="445" priority="562" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="444" priority="556" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="444" priority="563" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="443" priority="553" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="443" priority="560" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="442" priority="554" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="442" priority="561" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="441" priority="551" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="441" priority="558" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="440" priority="552" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="440" priority="559" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="439" priority="549" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="439" priority="556" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="438" priority="550" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="438" priority="557" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="437" priority="547" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="437" priority="554" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="436" priority="548" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="436" priority="555" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="435" priority="545" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="435" priority="552" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="434" priority="546" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="434" priority="553" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="433" priority="543" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="433" priority="550" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="432" priority="544" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="432" priority="551" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="431" priority="541" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="431" priority="548" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="430" priority="542" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="430" priority="549" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="429" priority="539" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="429" priority="546" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="428" priority="540" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="428" priority="547" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="427" priority="537" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="427" priority="544" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="426" priority="538" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="426" priority="545" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="425" priority="535" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="425" priority="542" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="424" priority="536" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="424" priority="543" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="423" priority="533" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="423" priority="540" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="422" priority="534" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="422" priority="541" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="421" priority="531" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="421" priority="538" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="420" priority="532" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="420" priority="539" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="419" priority="529" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="419" priority="536" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="418" priority="530" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="418" priority="537" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="417" priority="527" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="417" priority="534" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="416" priority="528" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="416" priority="535" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="415" priority="525" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="415" priority="532" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="414" priority="526" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="414" priority="533" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="413" priority="523" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="413" priority="530" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="412" priority="524" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="412" priority="531" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="411" priority="521" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="411" priority="528" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="410" priority="522" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="410" priority="529" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="409" priority="519" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="409" priority="526" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="408" priority="520" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="408" priority="527" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="407" priority="517" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="407" priority="524" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="406" priority="518" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="406" priority="525" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="405" priority="515" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="405" priority="522" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="404" priority="516" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="404" priority="523" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="403" priority="513" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="403" priority="520" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="402" priority="514" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="402" priority="521" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="401" priority="511" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="401" priority="518" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="400" priority="512" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="400" priority="519" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="399" priority="509" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="399" priority="516" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="398" priority="510" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="398" priority="517" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="397" priority="507" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="397" priority="514" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="396" priority="508" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="396" priority="515" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="395" priority="505" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="395" priority="512" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="394" priority="506" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="394" priority="513" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="393" priority="503" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="393" priority="510" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="392" priority="504" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="392" priority="511" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="391" priority="501" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="391" priority="508" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="390" priority="502" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="390" priority="509" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="389" priority="499" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="389" priority="506" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="388" priority="500" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="388" priority="507" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="387" priority="497" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="387" priority="504" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="386" priority="498" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="386" priority="505" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="385" priority="495" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="385" priority="502" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="384" priority="496" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="384" priority="503" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="383" priority="493" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="383" priority="500" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="382" priority="494" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="382" priority="501" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="381" priority="491" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="381" priority="498" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="380" priority="492" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="380" priority="499" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="379" priority="489" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="379" priority="496" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="378" priority="490" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="378" priority="497" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="377" priority="487" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="377" priority="494" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="376" priority="488" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="376" priority="495" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="375" priority="485" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="375" priority="492" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="374" priority="486" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="374" priority="493" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" dxfId="373" priority="366" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="373" priority="373" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="372" priority="367" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="372" priority="374" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",E35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:H7">
-    <cfRule type="containsText" dxfId="371" priority="364" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="371" priority="371" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="370" priority="365" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="370" priority="372" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="containsText" dxfId="369" priority="362" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="369" priority="369" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="368" priority="363" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="368" priority="370" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7:L7">
-    <cfRule type="containsText" dxfId="367" priority="360" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="367" priority="367" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="366" priority="361" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="366" priority="368" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="containsText" dxfId="365" priority="359" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="365" priority="366" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="containsText" dxfId="364" priority="357" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="364" priority="364" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="363" priority="358" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="363" priority="365" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="362" priority="355" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="362" priority="362" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="361" priority="356" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="361" priority="363" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="360" priority="353" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="360" priority="360" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="359" priority="354" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="359" priority="361" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="358" priority="351" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="358" priority="358" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="357" priority="352" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="357" priority="359" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="356" priority="349" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="356" priority="356" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="355" priority="350" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="355" priority="357" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="354" priority="347" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="354" priority="354" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="353" priority="348" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="353" priority="355" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="352" priority="345" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="352" priority="352" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="351" priority="346" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="351" priority="353" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="350" priority="343" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="350" priority="350" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="349" priority="344" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="349" priority="351" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="348" priority="341" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="348" priority="348" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="347" priority="342" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="347" priority="349" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="346" priority="339" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="346" priority="346" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="345" priority="340" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="345" priority="347" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="344" priority="337" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="344" priority="344" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="343" priority="338" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="343" priority="345" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="342" priority="335" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="342" priority="342" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="341" priority="336" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="341" priority="343" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="340" priority="333" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="340" priority="340" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="339" priority="334" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="339" priority="341" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="338" priority="331" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="338" priority="338" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="337" priority="332" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="337" priority="339" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="336" priority="329" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="336" priority="336" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="335" priority="330" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="335" priority="337" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="334" priority="327" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="334" priority="334" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="333" priority="328" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="333" priority="335" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="332" priority="325" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="332" priority="332" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="331" priority="326" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="331" priority="333" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="330" priority="323" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="330" priority="330" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="329" priority="324" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="329" priority="331" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="328" priority="321" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="328" priority="328" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="327" priority="322" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="327" priority="329" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="326" priority="319" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="326" priority="326" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="325" priority="320" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="325" priority="327" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="324" priority="317" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="324" priority="324" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="323" priority="318" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="323" priority="325" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="322" priority="315" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="322" priority="322" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="321" priority="316" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="321" priority="323" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="320" priority="313" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="320" priority="320" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="319" priority="314" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="319" priority="321" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="318" priority="311" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="318" priority="318" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="317" priority="312" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="317" priority="319" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="316" priority="309" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="316" priority="316" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="315" priority="310" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="315" priority="317" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="314" priority="307" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="314" priority="314" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="313" priority="308" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="313" priority="315" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="312" priority="305" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="312" priority="312" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="311" priority="306" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="311" priority="313" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="310" priority="303" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="310" priority="310" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="309" priority="304" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="309" priority="311" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="308" priority="301" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="308" priority="308" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="307" priority="302" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="307" priority="309" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="306" priority="299" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="306" priority="306" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="305" priority="300" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="305" priority="307" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="304" priority="297" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="304" priority="304" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="303" priority="298" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="303" priority="305" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="302" priority="295" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="302" priority="302" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="301" priority="296" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="301" priority="303" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="300" priority="293" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="300" priority="300" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="299" priority="294" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="299" priority="301" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="298" priority="291" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="298" priority="298" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="297" priority="292" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="297" priority="299" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="296" priority="289" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="296" priority="296" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="295" priority="290" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="295" priority="297" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="294" priority="287" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="294" priority="294" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="293" priority="288" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="293" priority="295" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="292" priority="285" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="292" priority="292" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="291" priority="286" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="291" priority="293" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="290" priority="283" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="290" priority="290" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="289" priority="284" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="289" priority="291" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="288" priority="281" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="288" priority="288" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="287" priority="282" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="287" priority="289" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="286" priority="279" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="286" priority="286" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="285" priority="280" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="285" priority="287" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="284" priority="277" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="284" priority="284" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="283" priority="278" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="283" priority="285" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="282" priority="275" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="282" priority="282" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="281" priority="276" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="281" priority="283" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="280" priority="273" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="280" priority="280" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="279" priority="274" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="279" priority="281" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="278" priority="271" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="278" priority="278" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="277" priority="272" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="277" priority="279" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="276" priority="269" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="276" priority="276" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="275" priority="270" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="275" priority="277" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="274" priority="267" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="274" priority="274" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="273" priority="268" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="273" priority="275" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="272" priority="265" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="272" priority="272" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="271" priority="266" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="271" priority="273" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="270" priority="263" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="270" priority="270" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="269" priority="264" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="269" priority="271" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="268" priority="261" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="268" priority="268" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="267" priority="262" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="267" priority="269" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="266" priority="259" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="266" priority="266" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="265" priority="260" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="265" priority="267" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="264" priority="257" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="264" priority="264" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="263" priority="258" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="263" priority="265" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="262" priority="255" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="262" priority="262" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="261" priority="256" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="261" priority="263" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="260" priority="253" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="260" priority="260" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="259" priority="254" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="259" priority="261" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="258" priority="251" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="258" priority="258" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="257" priority="252" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="257" priority="259" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="containsText" dxfId="256" priority="249" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="256" priority="256" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="255" priority="250" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="255" priority="257" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:H4">
-    <cfRule type="containsText" dxfId="254" priority="247" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="254" priority="254" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="253" priority="248" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="253" priority="255" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="containsText" dxfId="252" priority="245" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="252" priority="252" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="251" priority="246" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="251" priority="253" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:L4">
-    <cfRule type="containsText" dxfId="250" priority="243" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="250" priority="250" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="249" priority="244" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="249" priority="251" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="containsText" dxfId="248" priority="242" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="248" priority="249" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="containsText" dxfId="247" priority="240" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="247" priority="247" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="246" priority="241" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="246" priority="248" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="245" priority="238" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="245" priority="245" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="244" priority="239" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="244" priority="246" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="243" priority="236" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="243" priority="243" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="242" priority="237" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="242" priority="244" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="241" priority="234" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="241" priority="241" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="240" priority="235" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="240" priority="242" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="239" priority="232" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="239" priority="239" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="238" priority="233" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="238" priority="240" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="237" priority="230" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="237" priority="237" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="236" priority="231" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="236" priority="238" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="235" priority="228" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="235" priority="235" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="234" priority="229" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="234" priority="236" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="233" priority="226" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="233" priority="233" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="232" priority="227" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="232" priority="234" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="231" priority="224" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="231" priority="231" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="230" priority="225" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="230" priority="232" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="229" priority="222" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="229" priority="229" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="228" priority="223" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="228" priority="230" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="227" priority="220" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="227" priority="227" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="226" priority="221" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="226" priority="228" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="225" priority="218" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="225" priority="225" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="224" priority="219" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="224" priority="226" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="223" priority="216" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="223" priority="223" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="222" priority="217" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="222" priority="224" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="221" priority="214" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="221" priority="221" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="220" priority="215" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="220" priority="222" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="219" priority="212" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="219" priority="219" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="218" priority="213" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="218" priority="220" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="217" priority="210" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="217" priority="217" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="216" priority="211" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="216" priority="218" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="215" priority="208" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="215" priority="215" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="209" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="214" priority="216" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="213" priority="206" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="213" priority="213" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="212" priority="207" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="212" priority="214" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="211" priority="204" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="211" priority="211" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="205" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="210" priority="212" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="209" priority="202" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="209" priority="209" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="208" priority="203" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="208" priority="210" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="207" priority="200" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="207" priority="207" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="201" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="206" priority="208" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="205" priority="198" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="205" priority="205" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="199" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="204" priority="206" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="203" priority="196" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="203" priority="203" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="197" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="202" priority="204" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="201" priority="194" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="201" priority="201" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="200" priority="195" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="200" priority="202" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="199" priority="192" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="199" priority="199" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="193" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="198" priority="200" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="197" priority="190" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="197" priority="197" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="191" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="196" priority="198" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="195" priority="188" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="195" priority="195" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="189" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="194" priority="196" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="193" priority="186" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="193" priority="193" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="187" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="192" priority="194" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="191" priority="184" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="191" priority="191" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="185" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="190" priority="192" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="189" priority="182" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="189" priority="189" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="188" priority="183" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="188" priority="190" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="187" priority="180" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="187" priority="187" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="181" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="186" priority="188" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="185" priority="178" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="185" priority="185" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="179" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="184" priority="186" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="183" priority="176" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="183" priority="183" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="177" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="182" priority="184" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="181" priority="174" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="181" priority="181" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="175" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="180" priority="182" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="179" priority="172" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="179" priority="179" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="173" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="178" priority="180" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="177" priority="170" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="177" priority="177" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="176" priority="171" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="176" priority="178" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="175" priority="168" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="175" priority="175" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="169" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="174" priority="176" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="173" priority="166" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="173" priority="173" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="167" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="172" priority="174" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="171" priority="164" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="171" priority="171" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="165" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="170" priority="172" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="169" priority="162" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="169" priority="169" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="163" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="168" priority="170" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="167" priority="160" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="167" priority="167" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="161" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="166" priority="168" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="165" priority="158" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="165" priority="165" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="164" priority="159" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="164" priority="166" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="163" priority="156" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="163" priority="163" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="157" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="162" priority="164" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="161" priority="154" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="161" priority="161" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="155" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="160" priority="162" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="159" priority="152" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="159" priority="159" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="158" priority="153" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="158" priority="160" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="157" priority="150" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="157" priority="157" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="151" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="156" priority="158" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="155" priority="148" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="155" priority="155" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="149" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="154" priority="156" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="153" priority="146" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="153" priority="153" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="152" priority="147" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="152" priority="154" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="151" priority="144" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="151" priority="151" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="145" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="150" priority="152" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="149" priority="142" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="149" priority="149" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="143" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="148" priority="150" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="147" priority="140" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="147" priority="147" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="141" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="146" priority="148" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="145" priority="138" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="145" priority="145" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="139" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="144" priority="146" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="143" priority="136" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="143" priority="143" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="137" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="142" priority="144" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="141" priority="134" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="141" priority="141" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="135" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="140" priority="142" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="containsText" dxfId="139" priority="132" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="139" priority="139" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="133" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="138" priority="140" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:H8">
-    <cfRule type="containsText" dxfId="137" priority="130" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="137" priority="137" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="131" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="136" priority="138" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="containsText" dxfId="135" priority="128" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="135" priority="135" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",I8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="129" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="134" priority="136" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",I8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:L8">
-    <cfRule type="containsText" dxfId="133" priority="126" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="133" priority="133" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",K8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="127" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="132" priority="134" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",K8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="containsText" dxfId="131" priority="125" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="131" priority="132" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="containsText" dxfId="130" priority="123" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="130" priority="130" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="124" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="129" priority="131" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="128" priority="121" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="128" priority="128" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="122" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="127" priority="129" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="126" priority="119" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="126" priority="126" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="120" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="125" priority="127" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="124" priority="117" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="124" priority="124" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="118" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="123" priority="125" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="122" priority="115" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="122" priority="122" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="116" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="121" priority="123" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="120" priority="113" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="120" priority="120" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="114" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="119" priority="121" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="118" priority="111" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="118" priority="118" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="112" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="117" priority="119" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="116" priority="109" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="116" priority="116" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="110" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="115" priority="117" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="114" priority="107" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="114" priority="114" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="108" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="113" priority="115" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="112" priority="105" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="112" priority="112" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="106" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="111" priority="113" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="110" priority="103" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="110" priority="110" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="104" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="109" priority="111" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="108" priority="101" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="108" priority="108" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="102" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="107" priority="109" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="106" priority="99" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="106" priority="106" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="100" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="105" priority="107" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="104" priority="97" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="104" priority="104" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="98" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="103" priority="105" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="102" priority="95" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="102" priority="102" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="96" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="101" priority="103" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="100" priority="93" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="100" priority="100" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="94" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="99" priority="101" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="98" priority="91" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="98" priority="98" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="92" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="97" priority="99" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="96" priority="89" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="96" priority="96" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="90" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="95" priority="97" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="94" priority="87" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="94" priority="94" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="88" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="93" priority="95" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="92" priority="85" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="92" priority="92" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="86" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="91" priority="93" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="90" priority="83" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="90" priority="90" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="84" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="89" priority="91" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="88" priority="81" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="88" priority="88" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="82" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="87" priority="89" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="86" priority="79" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="86" priority="86" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="80" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="85" priority="87" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="84" priority="77" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="84" priority="84" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="78" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="83" priority="85" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="82" priority="75" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="82" priority="82" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="76" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="81" priority="83" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="80" priority="73" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="80" priority="80" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="74" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="79" priority="81" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="78" priority="71" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="78" priority="78" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="72" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="77" priority="79" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="76" priority="69" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="76" priority="76" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="70" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="75" priority="77" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="74" priority="67" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="74" priority="74" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="68" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="73" priority="75" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="72" priority="65" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="72" priority="72" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="66" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="71" priority="73" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="70" priority="63" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="70" priority="70" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="64" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="69" priority="71" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="68" priority="61" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="68" priority="68" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="62" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="67" priority="69" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="66" priority="59" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="60" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="65" priority="67" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="64" priority="57" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="64" priority="64" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="58" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="63" priority="65" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="62" priority="55" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="62" priority="62" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="56" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="61" priority="63" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="60" priority="53" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="60" priority="60" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="54" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="59" priority="61" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="58" priority="51" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="58" priority="58" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="52" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="57" priority="59" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="56" priority="49" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="56" priority="56" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="50" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="55" priority="57" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="54" priority="47" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="48" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="53" priority="55" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="52" priority="45" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="52" priority="52" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="46" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="51" priority="53" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="50" priority="43" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="50" priority="50" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="44" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="49" priority="51" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="48" priority="41" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="48" priority="48" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="42" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="47" priority="49" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="46" priority="39" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="46" priority="46" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="40" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="45" priority="47" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="44" priority="37" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="44" priority="44" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="38" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="43" priority="45" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="42" priority="35" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="36" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="40" priority="33" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="40" priority="40" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="34" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="39" priority="41" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="38" priority="31" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="32" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="36" priority="29" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="30" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="35" priority="37" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="34" priority="27" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="28" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="32" priority="25" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="26" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="30" priority="23" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="24" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="28" priority="21" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="28" priority="28" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="22" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="26" priority="19" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="24" priority="17" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="18" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:I9">
-    <cfRule type="containsText" dxfId="20" priority="13" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="14" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:L9 D9">
-    <cfRule type="containsText" dxfId="18" priority="11" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="12" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="containsText" dxfId="16" priority="10" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="9" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11:I11">
-    <cfRule type="containsText" dxfId="13" priority="6" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:L11 D11">
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="Sim">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="Sim">
       <formula>NOT(ISERROR(SEARCH("Sim",D11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="Não">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Não">
       <formula>NOT(ISERROR(SEARCH("Não",D11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Android">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="Android">
       <formula>NOT(ISERROR(SEARCH("Android",J11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Web">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="Web">
       <formula>NOT(ISERROR(SEARCH("Web",J11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="iOS">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="iOS">
       <formula>NOT(ISERROR(SEARCH("iOS",J11)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F12:I12">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",F12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",F12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12:L12 D12">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Sim">
+      <formula>NOT(ISERROR(SEARCH("Sim",D12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Não">
+      <formula>NOT(ISERROR(SEARCH("Não",D12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Android">
+      <formula>NOT(ISERROR(SEARCH("Android",J12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Web">
+      <formula>NOT(ISERROR(SEARCH("Web",J12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="iOS">
+      <formula>NOT(ISERROR(SEARCH("iOS",J12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K44:L46 K48:L50 D54:D60 K54:L60 K62:L67 K69:L73 D69:D73 D62:D67 D2:D50 K2:L42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K44:L46 K48:L50 D54:D60 K54:L60 K62:L67 K69:L73 D69:D73 D62:D67 K2:L42 D2:D50">
       <formula1>"Sim,Não"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J54:J60 J69:J73 J62:J67 J2:J50">
@@ -19850,16 +19961,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="37" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5703125" style="37" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" style="37" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="15.85546875" style="37" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.28515625" style="37" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="1.5703125" style="37" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.85546875" style="37" customWidth="1" collapsed="1"/>
-    <col min="9" max="12" width="13.42578125" style="37" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="1.5703125" style="37" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="9.140625" style="37" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="37" width="1.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="37" width="14.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="37" width="15.85546875" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" style="37" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="37" width="19.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="37" width="1.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="37" width="15.85546875" collapsed="true"/>
+    <col min="9" max="12" customWidth="true" style="37" width="13.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="37" width="1.5703125" collapsed="true"/>
+    <col min="14" max="16384" style="37" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="7.5" customHeight="1">
@@ -19986,11 +20097,11 @@
       </c>
       <c r="I7" s="39">
         <f>COUNTIF(Testes!J3:J51,"Android")</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J7" s="39">
         <f>COUNTIFS(Testes!G3:G51,"Passed",Testes!J3:J51,"Android")</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K7" s="39">
         <f>COUNTIFS(Testes!G3:G51,"Failed",Testes!J3:J51,"Android")</f>
@@ -20005,7 +20116,7 @@
       <c r="A8" s="44"/>
       <c r="B8" s="53">
         <f>COUNTIF(Testes!A3:A51,"&lt;&gt;"&amp;"")</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" s="113"/>
       <c r="D8" s="113"/>
@@ -20072,7 +20183,7 @@
       </c>
       <c r="D10" s="39">
         <f>J11</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" s="39">
         <f>K11</f>
@@ -20108,11 +20219,11 @@
       </c>
       <c r="I11" s="39">
         <f>SUM(I7:I9)</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J11" s="39">
         <f>SUM(J7:J9)</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K11" s="39">
         <f>SUM(K7:K9)</f>
@@ -20203,9 +20314,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -20358,29 +20469,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" style="9" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.85546875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.5703125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.140625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.5703125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.28515625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.5703125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.85546875" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8.5703125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="3.42578125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.5703125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.5703125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="24.5703125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.85546875" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.85546875" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="20.140625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="20.42578125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="16384" width="9.140625" style="13" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="9" width="35.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="9" width="9.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="9" width="7.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="9" width="25.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="13" width="12.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="13" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="13" width="21.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="13" width="19.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="13" width="15.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="13" width="20.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="13" width="13.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="13" width="19.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="13" width="8.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="13" width="3.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="13" width="18.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="13" width="13.5703125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="13" width="12.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="13" width="24.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="13" width="13.85546875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="13" width="11.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="13" width="20.140625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="13" width="20.42578125" collapsed="true"/>
+    <col min="23" max="16384" style="13" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="12" customFormat="1">
@@ -20834,11 +20945,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">

</xml_diff>